<commit_message>
Done with the testing
</commit_message>
<xml_diff>
--- a/backend/src/file/example_files/dummy_file.xlsx
+++ b/backend/src/file/example_files/dummy_file.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roysegall/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/financeular/backend/src/file/example_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF56099A-19C5-8A4D-89BD-66A17686CA0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843D33C3-545C-0843-B2D0-47966858985F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20980" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="276">
   <si>
     <t>כמה נכנס כסף בפועל</t>
   </si>
@@ -1370,7 +1370,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" ht="18">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -1406,7 +1406,7 @@
       <c r="T2" s="37"/>
       <c r="U2" s="6"/>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" ht="18">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="E3" s="7"/>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="U3" s="6"/>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" ht="18">
       <c r="A4" s="7"/>
       <c r="B4" s="2" t="s">
         <v>13</v>
@@ -1496,7 +1496,7 @@
       <c r="T4" s="24"/>
       <c r="U4" s="25"/>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" ht="18">
       <c r="A5" s="26"/>
       <c r="B5" s="2" t="s">
         <v>17</v>
@@ -1549,7 +1549,7 @@
       </c>
       <c r="U5" s="25"/>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" ht="18">
       <c r="B6" s="8"/>
       <c r="F6" s="16">
         <v>0</v>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="U6" s="25"/>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" ht="18">
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
@@ -1642,7 +1642,7 @@
       </c>
       <c r="U7" s="25"/>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" ht="18">
       <c r="B8" s="8"/>
       <c r="F8" s="16"/>
       <c r="G8" s="28"/>
@@ -1678,7 +1678,7 @@
       </c>
       <c r="U8" s="25"/>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" ht="18">
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
@@ -1723,7 +1723,7 @@
       </c>
       <c r="U9" s="25"/>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" ht="18">
       <c r="B10" s="8"/>
       <c r="F10" s="16"/>
       <c r="G10" s="28"/>
@@ -1759,7 +1759,7 @@
       </c>
       <c r="U10" s="25"/>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" ht="18">
       <c r="B11" s="2" t="s">
         <v>41</v>
       </c>
@@ -1806,7 +1806,7 @@
       </c>
       <c r="U11" s="25"/>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" ht="18">
       <c r="F12" s="16"/>
       <c r="G12" s="28"/>
       <c r="H12" s="5"/>
@@ -1841,7 +1841,7 @@
       </c>
       <c r="U12" s="25"/>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" ht="18">
       <c r="F13" s="16"/>
       <c r="G13" s="28"/>
       <c r="H13" s="5"/>
@@ -1876,7 +1876,7 @@
       </c>
       <c r="U13" s="25"/>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" ht="18">
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -1900,7 +1900,7 @@
       </c>
       <c r="U14" s="25"/>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" ht="18">
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -1924,7 +1924,7 @@
       </c>
       <c r="U15" s="25"/>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" ht="18">
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -1948,7 +1948,7 @@
       </c>
       <c r="U16" s="25"/>
     </row>
-    <row r="17" spans="6:21">
+    <row r="17" spans="6:21" ht="18">
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -1972,7 +1972,7 @@
       </c>
       <c r="U17" s="25"/>
     </row>
-    <row r="18" spans="6:21">
+    <row r="18" spans="6:21" ht="18">
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
@@ -1996,7 +1996,7 @@
       </c>
       <c r="U18" s="25"/>
     </row>
-    <row r="19" spans="6:21">
+    <row r="19" spans="6:21" ht="18">
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -2020,7 +2020,7 @@
       </c>
       <c r="U19" s="25"/>
     </row>
-    <row r="20" spans="6:21">
+    <row r="20" spans="6:21" ht="18">
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
@@ -2044,7 +2044,7 @@
       </c>
       <c r="U20" s="25"/>
     </row>
-    <row r="21" spans="6:21">
+    <row r="21" spans="6:21" ht="18">
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="U21" s="25"/>
     </row>
-    <row r="22" spans="6:21">
+    <row r="22" spans="6:21" ht="18">
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
@@ -2086,7 +2086,7 @@
       </c>
       <c r="U22" s="25"/>
     </row>
-    <row r="23" spans="6:21">
+    <row r="23" spans="6:21" ht="18">
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
@@ -2107,7 +2107,7 @@
       </c>
       <c r="U23" s="25"/>
     </row>
-    <row r="24" spans="6:21">
+    <row r="24" spans="6:21" ht="18">
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
@@ -2128,7 +2128,7 @@
       </c>
       <c r="U24" s="25"/>
     </row>
-    <row r="25" spans="6:21">
+    <row r="25" spans="6:21" ht="18">
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
@@ -2149,7 +2149,7 @@
       </c>
       <c r="U25" s="25"/>
     </row>
-    <row r="26" spans="6:21">
+    <row r="26" spans="6:21" ht="18">
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
@@ -2170,7 +2170,7 @@
       </c>
       <c r="U26" s="25"/>
     </row>
-    <row r="27" spans="6:21">
+    <row r="27" spans="6:21" ht="18">
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
@@ -2191,7 +2191,7 @@
       </c>
       <c r="U27" s="25"/>
     </row>
-    <row r="28" spans="6:21">
+    <row r="28" spans="6:21" ht="18">
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
@@ -2212,7 +2212,7 @@
       </c>
       <c r="U28" s="25"/>
     </row>
-    <row r="29" spans="6:21">
+    <row r="29" spans="6:21" ht="18">
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
@@ -2233,7 +2233,7 @@
       </c>
       <c r="U29" s="25"/>
     </row>
-    <row r="30" spans="6:21">
+    <row r="30" spans="6:21" ht="18">
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
@@ -2254,7 +2254,7 @@
       </c>
       <c r="U30" s="25"/>
     </row>
-    <row r="31" spans="6:21">
+    <row r="31" spans="6:21" ht="18">
       <c r="F31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="U31" s="25"/>
     </row>
-    <row r="32" spans="6:21">
+    <row r="32" spans="6:21" ht="18">
       <c r="R32" s="22">
         <v>1000</v>
       </c>
@@ -2289,7 +2289,7 @@
       </c>
       <c r="U32" s="25"/>
     </row>
-    <row r="33" spans="18:21">
+    <row r="33" spans="18:21" ht="18">
       <c r="R33" s="22">
         <v>40</v>
       </c>
@@ -2301,7 +2301,7 @@
       </c>
       <c r="U33" s="25"/>
     </row>
-    <row r="34" spans="18:21">
+    <row r="34" spans="18:21" ht="18">
       <c r="R34" s="22">
         <v>38</v>
       </c>
@@ -2313,7 +2313,7 @@
       </c>
       <c r="U34" s="25"/>
     </row>
-    <row r="35" spans="18:21">
+    <row r="35" spans="18:21" ht="18">
       <c r="R35" s="22">
         <v>124</v>
       </c>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="U35" s="25"/>
     </row>
-    <row r="36" spans="18:21">
+    <row r="36" spans="18:21" ht="18">
       <c r="R36" s="22">
         <v>70</v>
       </c>
@@ -2337,7 +2337,7 @@
       </c>
       <c r="U36" s="25"/>
     </row>
-    <row r="37" spans="18:21">
+    <row r="37" spans="18:21" ht="18">
       <c r="R37" s="22">
         <v>59</v>
       </c>
@@ -2349,7 +2349,7 @@
       </c>
       <c r="U37" s="25"/>
     </row>
-    <row r="38" spans="18:21">
+    <row r="38" spans="18:21" ht="18">
       <c r="R38" s="22">
         <v>40</v>
       </c>
@@ -2361,7 +2361,7 @@
       </c>
       <c r="U38" s="25"/>
     </row>
-    <row r="39" spans="18:21">
+    <row r="39" spans="18:21" ht="18">
       <c r="R39" s="22">
         <v>75</v>
       </c>
@@ -2373,7 +2373,7 @@
       </c>
       <c r="U39" s="25"/>
     </row>
-    <row r="40" spans="18:21">
+    <row r="40" spans="18:21" ht="18">
       <c r="R40" s="22">
         <v>36</v>
       </c>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="U40" s="25"/>
     </row>
-    <row r="41" spans="18:21">
+    <row r="41" spans="18:21" ht="18">
       <c r="R41" s="22">
         <v>70.12</v>
       </c>
@@ -2397,7 +2397,7 @@
       </c>
       <c r="U41" s="25"/>
     </row>
-    <row r="42" spans="18:21">
+    <row r="42" spans="18:21" ht="18">
       <c r="R42" s="22">
         <v>200</v>
       </c>
@@ -2409,7 +2409,7 @@
       </c>
       <c r="U42" s="25"/>
     </row>
-    <row r="43" spans="18:21">
+    <row r="43" spans="18:21" ht="18">
       <c r="R43" s="22">
         <v>602</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="18:21">
+    <row r="44" spans="18:21" ht="18">
       <c r="R44" s="22">
         <v>55</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="18:21">
+    <row r="45" spans="18:21" ht="18">
       <c r="R45" s="22">
         <v>50</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="46" spans="18:21">
+    <row r="46" spans="18:21" ht="18">
       <c r="R46" s="22">
         <v>59</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="47" spans="18:21">
+    <row r="47" spans="18:21" ht="18">
       <c r="R47" s="22">
         <v>479</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="48" spans="18:21">
+    <row r="48" spans="18:21" ht="18">
       <c r="R48" s="22">
         <v>79</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="49" spans="18:20">
+    <row r="49" spans="18:20" ht="18">
       <c r="R49" s="22">
         <v>50</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="18:20">
+    <row r="50" spans="18:20" ht="18">
       <c r="R50" s="22">
         <v>109</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="51" spans="18:20">
+    <row r="51" spans="18:20" ht="18">
       <c r="R51" s="22">
         <v>66.12</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="18:20">
+    <row r="52" spans="18:20" ht="18">
       <c r="R52" s="22">
         <v>50</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="18:20">
+    <row r="53" spans="18:20" ht="18">
       <c r="R53" s="22">
         <v>360</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="18:20">
+    <row r="54" spans="18:20" ht="18">
       <c r="R54" s="22">
         <v>60</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="55" spans="18:20">
+    <row r="55" spans="18:20" ht="18">
       <c r="R55" s="22">
         <v>50</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="18:20">
+    <row r="56" spans="18:20" ht="18">
       <c r="R56" s="22">
         <v>20</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="57" spans="18:20">
+    <row r="57" spans="18:20" ht="18">
       <c r="R57" s="22">
         <v>22</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="18:20">
+    <row r="58" spans="18:20" ht="18">
       <c r="R58" s="22">
         <v>21</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="18:20">
+    <row r="59" spans="18:20" ht="18">
       <c r="R59" s="22">
         <v>45</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="18:20">
+    <row r="60" spans="18:20" ht="18">
       <c r="R60" s="22">
         <v>89</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="18:20">
+    <row r="61" spans="18:20" ht="18">
       <c r="R61" s="22">
         <v>105</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="18:20">
+    <row r="62" spans="18:20" ht="18">
       <c r="R62" s="22">
         <v>40</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="63" spans="18:20">
+    <row r="63" spans="18:20" ht="18">
       <c r="R63" s="22">
         <v>36</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="64" spans="18:20">
+    <row r="64" spans="18:20" ht="18">
       <c r="R64" s="22">
         <v>20</v>
       </c>
@@ -2651,12 +2651,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="65" spans="18:20">
+    <row r="65" spans="18:20" ht="18">
       <c r="R65" s="22"/>
       <c r="S65" s="29"/>
       <c r="T65" s="24"/>
     </row>
-    <row r="66" spans="18:20">
+    <row r="66" spans="18:20" ht="18">
       <c r="R66" s="22"/>
       <c r="S66" s="29"/>
       <c r="T66" s="24"/>
@@ -2744,7 +2744,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" ht="18">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -2780,7 +2780,7 @@
       <c r="T2" s="37"/>
       <c r="U2" s="6"/>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" ht="18">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="E3" s="7"/>
@@ -2823,7 +2823,7 @@
       </c>
       <c r="U3" s="6"/>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" ht="18">
       <c r="A4" s="7"/>
       <c r="B4" s="2" t="s">
         <v>13</v>
@@ -2870,7 +2870,7 @@
       <c r="T4" s="24"/>
       <c r="U4" s="25"/>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" ht="18">
       <c r="A5" s="26"/>
       <c r="B5" s="2" t="s">
         <v>17</v>
@@ -2923,7 +2923,7 @@
       </c>
       <c r="U5" s="25"/>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" ht="18">
       <c r="B6" s="8"/>
       <c r="F6" s="16">
         <v>10000</v>
@@ -2965,7 +2965,7 @@
       </c>
       <c r="U6" s="25"/>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" ht="18">
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
@@ -3012,7 +3012,7 @@
       </c>
       <c r="U7" s="25"/>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" ht="18">
       <c r="B8" s="8"/>
       <c r="F8" s="16"/>
       <c r="G8" s="28"/>
@@ -3048,7 +3048,7 @@
       </c>
       <c r="U8" s="25"/>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" ht="18">
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
@@ -3093,7 +3093,7 @@
       </c>
       <c r="U9" s="25"/>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" ht="18">
       <c r="B10" s="8"/>
       <c r="F10" s="16"/>
       <c r="G10" s="28"/>
@@ -3129,7 +3129,7 @@
       </c>
       <c r="U10" s="25"/>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" ht="18">
       <c r="B11" s="2" t="s">
         <v>41</v>
       </c>
@@ -3176,7 +3176,7 @@
       </c>
       <c r="U11" s="25"/>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" ht="18">
       <c r="F12" s="16"/>
       <c r="G12" s="28"/>
       <c r="H12" s="5"/>
@@ -3211,7 +3211,7 @@
       </c>
       <c r="U12" s="25"/>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" ht="18">
       <c r="F13" s="16"/>
       <c r="G13" s="28"/>
       <c r="H13" s="5"/>
@@ -3246,7 +3246,7 @@
       </c>
       <c r="U13" s="25"/>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" ht="18">
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -3270,7 +3270,7 @@
       </c>
       <c r="U14" s="25"/>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" ht="18">
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -3294,7 +3294,7 @@
       </c>
       <c r="U15" s="25"/>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" ht="18">
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -3318,7 +3318,7 @@
       </c>
       <c r="U16" s="25"/>
     </row>
-    <row r="17" spans="6:21">
+    <row r="17" spans="6:21" ht="18">
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -3342,7 +3342,7 @@
       </c>
       <c r="U17" s="25"/>
     </row>
-    <row r="18" spans="6:21">
+    <row r="18" spans="6:21" ht="18">
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
@@ -3366,7 +3366,7 @@
       </c>
       <c r="U18" s="25"/>
     </row>
-    <row r="19" spans="6:21">
+    <row r="19" spans="6:21" ht="18">
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -3390,7 +3390,7 @@
       </c>
       <c r="U19" s="25"/>
     </row>
-    <row r="20" spans="6:21">
+    <row r="20" spans="6:21" ht="18">
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
@@ -3414,7 +3414,7 @@
       </c>
       <c r="U20" s="25"/>
     </row>
-    <row r="21" spans="6:21">
+    <row r="21" spans="6:21" ht="18">
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
@@ -3435,7 +3435,7 @@
       </c>
       <c r="U21" s="25"/>
     </row>
-    <row r="22" spans="6:21">
+    <row r="22" spans="6:21" ht="18">
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
@@ -3456,7 +3456,7 @@
       </c>
       <c r="U22" s="25"/>
     </row>
-    <row r="23" spans="6:21">
+    <row r="23" spans="6:21" ht="18">
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
@@ -3477,7 +3477,7 @@
       </c>
       <c r="U23" s="25"/>
     </row>
-    <row r="24" spans="6:21">
+    <row r="24" spans="6:21" ht="18">
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
@@ -3498,7 +3498,7 @@
       </c>
       <c r="U24" s="25"/>
     </row>
-    <row r="25" spans="6:21">
+    <row r="25" spans="6:21" ht="18">
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
@@ -3519,7 +3519,7 @@
       </c>
       <c r="U25" s="25"/>
     </row>
-    <row r="26" spans="6:21">
+    <row r="26" spans="6:21" ht="18">
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
@@ -3540,7 +3540,7 @@
       </c>
       <c r="U26" s="25"/>
     </row>
-    <row r="27" spans="6:21">
+    <row r="27" spans="6:21" ht="18">
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
@@ -3561,7 +3561,7 @@
       </c>
       <c r="U27" s="25"/>
     </row>
-    <row r="28" spans="6:21">
+    <row r="28" spans="6:21" ht="18">
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="U28" s="25"/>
     </row>
-    <row r="29" spans="6:21">
+    <row r="29" spans="6:21" ht="18">
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
@@ -3603,7 +3603,7 @@
       </c>
       <c r="U29" s="25"/>
     </row>
-    <row r="30" spans="6:21">
+    <row r="30" spans="6:21" ht="18">
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
@@ -3624,7 +3624,7 @@
       </c>
       <c r="U30" s="25"/>
     </row>
-    <row r="31" spans="6:21">
+    <row r="31" spans="6:21" ht="18">
       <c r="F31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -3647,7 +3647,7 @@
       </c>
       <c r="U31" s="25"/>
     </row>
-    <row r="32" spans="6:21">
+    <row r="32" spans="6:21" ht="18">
       <c r="R32" s="22">
         <v>80</v>
       </c>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="U32" s="25"/>
     </row>
-    <row r="33" spans="18:21">
+    <row r="33" spans="18:21" ht="18">
       <c r="R33" s="22">
         <v>170</v>
       </c>
@@ -3671,7 +3671,7 @@
       </c>
       <c r="U33" s="25"/>
     </row>
-    <row r="34" spans="18:21">
+    <row r="34" spans="18:21" ht="18">
       <c r="R34" s="22">
         <v>69</v>
       </c>
@@ -3683,7 +3683,7 @@
       </c>
       <c r="U34" s="25"/>
     </row>
-    <row r="35" spans="18:21">
+    <row r="35" spans="18:21" ht="18">
       <c r="R35" s="22">
         <v>100</v>
       </c>
@@ -3695,7 +3695,7 @@
       </c>
       <c r="U35" s="25"/>
     </row>
-    <row r="36" spans="18:21">
+    <row r="36" spans="18:21" ht="18">
       <c r="R36" s="22">
         <v>390</v>
       </c>
@@ -3707,7 +3707,7 @@
       </c>
       <c r="U36" s="25"/>
     </row>
-    <row r="37" spans="18:21">
+    <row r="37" spans="18:21" ht="18">
       <c r="R37" s="22">
         <v>4700</v>
       </c>
@@ -3719,7 +3719,7 @@
       </c>
       <c r="U37" s="25"/>
     </row>
-    <row r="38" spans="18:21">
+    <row r="38" spans="18:21" ht="18">
       <c r="R38" s="22">
         <v>79</v>
       </c>
@@ -3731,7 +3731,7 @@
       </c>
       <c r="U38" s="25"/>
     </row>
-    <row r="39" spans="18:21">
+    <row r="39" spans="18:21" ht="18">
       <c r="R39" s="22">
         <v>30</v>
       </c>
@@ -3743,7 +3743,7 @@
       </c>
       <c r="U39" s="25"/>
     </row>
-    <row r="40" spans="18:21">
+    <row r="40" spans="18:21" ht="18">
       <c r="R40" s="22">
         <v>365</v>
       </c>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="U40" s="25"/>
     </row>
-    <row r="41" spans="18:21">
+    <row r="41" spans="18:21" ht="18">
       <c r="R41" s="22">
         <v>85</v>
       </c>
@@ -3767,7 +3767,7 @@
       </c>
       <c r="U41" s="25"/>
     </row>
-    <row r="42" spans="18:21">
+    <row r="42" spans="18:21" ht="18">
       <c r="R42" s="22">
         <v>132</v>
       </c>
@@ -3779,7 +3779,7 @@
       </c>
       <c r="U42" s="25"/>
     </row>
-    <row r="43" spans="18:21">
+    <row r="43" spans="18:21" ht="18">
       <c r="R43" s="22">
         <v>53</v>
       </c>
@@ -3790,7 +3790,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="44" spans="18:21">
+    <row r="44" spans="18:21" ht="18">
       <c r="R44" s="22">
         <v>44</v>
       </c>
@@ -3801,7 +3801,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="45" spans="18:21">
+    <row r="45" spans="18:21" ht="18">
       <c r="R45" s="22">
         <v>180</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="46" spans="18:21">
+    <row r="46" spans="18:21" ht="18">
       <c r="R46" s="22">
         <v>178</v>
       </c>
@@ -3823,7 +3823,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="47" spans="18:21">
+    <row r="47" spans="18:21" ht="18">
       <c r="R47" s="22">
         <v>55</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="18:21">
+    <row r="48" spans="18:21" ht="18">
       <c r="R48" s="22">
         <v>40</v>
       </c>
@@ -3845,7 +3845,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="18:20">
+    <row r="49" spans="18:20" ht="18">
       <c r="R49" s="22">
         <v>80</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="50" spans="18:20">
+    <row r="50" spans="18:20" ht="18">
       <c r="R50" s="22">
         <v>90</v>
       </c>
@@ -3867,7 +3867,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="51" spans="18:20">
+    <row r="51" spans="18:20" ht="18">
       <c r="R51" s="22">
         <v>50</v>
       </c>
@@ -3878,7 +3878,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="52" spans="18:20">
+    <row r="52" spans="18:20" ht="18">
       <c r="R52" s="22">
         <v>161</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="53" spans="18:20">
+    <row r="53" spans="18:20" ht="18">
       <c r="R53" s="22">
         <v>400</v>
       </c>
@@ -3900,7 +3900,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="54" spans="18:20">
+    <row r="54" spans="18:20" ht="18">
       <c r="R54" s="22">
         <v>80</v>
       </c>
@@ -3911,7 +3911,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="55" spans="18:20">
+    <row r="55" spans="18:20" ht="18">
       <c r="R55" s="22">
         <v>375</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="18:20">
+    <row r="56" spans="18:20" ht="18">
       <c r="R56" s="22">
         <v>88</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="18:20">
+    <row r="57" spans="18:20" ht="18">
       <c r="R57" s="22">
         <v>50</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="58" spans="18:20">
+    <row r="58" spans="18:20" ht="18">
       <c r="R58" s="22">
         <v>430</v>
       </c>
@@ -3953,22 +3953,22 @@
         <v>135</v>
       </c>
     </row>
-    <row r="59" spans="18:20">
+    <row r="59" spans="18:20" ht="18">
       <c r="R59" s="22"/>
       <c r="S59" s="29"/>
       <c r="T59" s="24"/>
     </row>
-    <row r="60" spans="18:20">
+    <row r="60" spans="18:20" ht="18">
       <c r="R60" s="22"/>
       <c r="S60" s="29"/>
       <c r="T60" s="24"/>
     </row>
-    <row r="61" spans="18:20">
+    <row r="61" spans="18:20" ht="18">
       <c r="R61" s="22"/>
       <c r="S61" s="29"/>
       <c r="T61" s="24"/>
     </row>
-    <row r="62" spans="18:20">
+    <row r="62" spans="18:20" ht="18">
       <c r="R62" s="22"/>
       <c r="S62" s="29"/>
       <c r="T62" s="24"/>
@@ -4031,7 +4031,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" ht="18">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -4067,7 +4067,7 @@
       <c r="T2" s="37"/>
       <c r="U2" s="6"/>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" ht="18">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="E3" s="7"/>
@@ -4110,7 +4110,7 @@
       </c>
       <c r="U3" s="6"/>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" ht="18">
       <c r="A4" s="7"/>
       <c r="B4" s="2" t="s">
         <v>13</v>
@@ -4157,7 +4157,7 @@
       <c r="T4" s="24"/>
       <c r="U4" s="25"/>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" ht="18">
       <c r="A5" s="26"/>
       <c r="B5" s="2" t="s">
         <v>17</v>
@@ -4210,7 +4210,7 @@
       </c>
       <c r="U5" s="25"/>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" ht="18">
       <c r="B6" s="8"/>
       <c r="F6" s="16"/>
       <c r="G6" s="17"/>
@@ -4248,7 +4248,7 @@
       </c>
       <c r="U6" s="25"/>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" ht="18">
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
@@ -4295,7 +4295,7 @@
       </c>
       <c r="U7" s="25"/>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" ht="18">
       <c r="B8" s="8"/>
       <c r="F8" s="16"/>
       <c r="G8" s="28"/>
@@ -4331,7 +4331,7 @@
       </c>
       <c r="U8" s="25"/>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" ht="18">
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
@@ -4376,7 +4376,7 @@
       </c>
       <c r="U9" s="25"/>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" ht="18">
       <c r="B10" s="8"/>
       <c r="F10" s="16"/>
       <c r="G10" s="28"/>
@@ -4412,7 +4412,7 @@
       </c>
       <c r="U10" s="25"/>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" ht="18">
       <c r="B11" s="2" t="s">
         <v>41</v>
       </c>
@@ -4459,7 +4459,7 @@
       </c>
       <c r="U11" s="25"/>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" ht="18">
       <c r="F12" s="16"/>
       <c r="G12" s="28"/>
       <c r="H12" s="5"/>
@@ -4494,7 +4494,7 @@
       </c>
       <c r="U12" s="25"/>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" ht="18">
       <c r="F13" s="16"/>
       <c r="G13" s="28"/>
       <c r="H13" s="5"/>
@@ -4529,7 +4529,7 @@
       </c>
       <c r="U13" s="25"/>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" ht="18">
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -4553,7 +4553,7 @@
       </c>
       <c r="U14" s="25"/>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" ht="18">
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -4577,7 +4577,7 @@
       </c>
       <c r="U15" s="25"/>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" ht="18">
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -4601,7 +4601,7 @@
       </c>
       <c r="U16" s="25"/>
     </row>
-    <row r="17" spans="6:21">
+    <row r="17" spans="6:21" ht="18">
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -4625,7 +4625,7 @@
       </c>
       <c r="U17" s="25"/>
     </row>
-    <row r="18" spans="6:21">
+    <row r="18" spans="6:21" ht="18">
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
@@ -4649,7 +4649,7 @@
       </c>
       <c r="U18" s="25"/>
     </row>
-    <row r="19" spans="6:21">
+    <row r="19" spans="6:21" ht="18">
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -4673,7 +4673,7 @@
       </c>
       <c r="U19" s="25"/>
     </row>
-    <row r="20" spans="6:21">
+    <row r="20" spans="6:21" ht="18">
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
@@ -4697,7 +4697,7 @@
       </c>
       <c r="U20" s="25"/>
     </row>
-    <row r="21" spans="6:21">
+    <row r="21" spans="6:21" ht="18">
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
@@ -4718,7 +4718,7 @@
       </c>
       <c r="U21" s="25"/>
     </row>
-    <row r="22" spans="6:21">
+    <row r="22" spans="6:21" ht="18">
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
@@ -4739,7 +4739,7 @@
       </c>
       <c r="U22" s="25"/>
     </row>
-    <row r="23" spans="6:21">
+    <row r="23" spans="6:21" ht="18">
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
@@ -4760,7 +4760,7 @@
       </c>
       <c r="U23" s="25"/>
     </row>
-    <row r="24" spans="6:21">
+    <row r="24" spans="6:21" ht="18">
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
@@ -4781,7 +4781,7 @@
       </c>
       <c r="U24" s="25"/>
     </row>
-    <row r="25" spans="6:21">
+    <row r="25" spans="6:21" ht="18">
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
@@ -4802,7 +4802,7 @@
       </c>
       <c r="U25" s="25"/>
     </row>
-    <row r="26" spans="6:21">
+    <row r="26" spans="6:21" ht="18">
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
@@ -4823,7 +4823,7 @@
       </c>
       <c r="U26" s="25"/>
     </row>
-    <row r="27" spans="6:21">
+    <row r="27" spans="6:21" ht="18">
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
@@ -4844,7 +4844,7 @@
       </c>
       <c r="U27" s="25"/>
     </row>
-    <row r="28" spans="6:21">
+    <row r="28" spans="6:21" ht="18">
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
@@ -4865,7 +4865,7 @@
       </c>
       <c r="U28" s="25"/>
     </row>
-    <row r="29" spans="6:21">
+    <row r="29" spans="6:21" ht="18">
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
@@ -4886,7 +4886,7 @@
       </c>
       <c r="U29" s="25"/>
     </row>
-    <row r="30" spans="6:21">
+    <row r="30" spans="6:21" ht="18">
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
@@ -4907,7 +4907,7 @@
       </c>
       <c r="U30" s="25"/>
     </row>
-    <row r="31" spans="6:21">
+    <row r="31" spans="6:21" ht="18">
       <c r="F31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -4930,7 +4930,7 @@
       </c>
       <c r="U31" s="25"/>
     </row>
-    <row r="32" spans="6:21">
+    <row r="32" spans="6:21" ht="18">
       <c r="R32" s="22">
         <v>600</v>
       </c>
@@ -4940,7 +4940,7 @@
       </c>
       <c r="U32" s="25"/>
     </row>
-    <row r="33" spans="18:21">
+    <row r="33" spans="18:21" ht="18">
       <c r="R33" s="22"/>
       <c r="S33" s="23"/>
       <c r="T33" s="24" t="s">
@@ -4948,7 +4948,7 @@
       </c>
       <c r="U33" s="25"/>
     </row>
-    <row r="34" spans="18:21">
+    <row r="34" spans="18:21" ht="18">
       <c r="R34" s="22">
         <v>500</v>
       </c>
@@ -4958,150 +4958,150 @@
       </c>
       <c r="U34" s="25"/>
     </row>
-    <row r="35" spans="18:21">
+    <row r="35" spans="18:21" ht="18">
       <c r="R35" s="22"/>
       <c r="S35" s="29"/>
       <c r="T35" s="24"/>
       <c r="U35" s="25"/>
     </row>
-    <row r="36" spans="18:21">
+    <row r="36" spans="18:21" ht="18">
       <c r="R36" s="22"/>
       <c r="S36" s="29"/>
       <c r="T36" s="24"/>
       <c r="U36" s="25"/>
     </row>
-    <row r="37" spans="18:21">
+    <row r="37" spans="18:21" ht="18">
       <c r="R37" s="22"/>
       <c r="S37" s="29"/>
       <c r="T37" s="24"/>
       <c r="U37" s="25"/>
     </row>
-    <row r="38" spans="18:21">
+    <row r="38" spans="18:21" ht="18">
       <c r="R38" s="22"/>
       <c r="S38" s="29"/>
       <c r="T38" s="24"/>
       <c r="U38" s="25"/>
     </row>
-    <row r="39" spans="18:21">
+    <row r="39" spans="18:21" ht="18">
       <c r="R39" s="22"/>
       <c r="S39" s="29"/>
       <c r="T39" s="24"/>
       <c r="U39" s="25"/>
     </row>
-    <row r="40" spans="18:21">
+    <row r="40" spans="18:21" ht="18">
       <c r="R40" s="22"/>
       <c r="S40" s="29"/>
       <c r="T40" s="24"/>
       <c r="U40" s="25"/>
     </row>
-    <row r="41" spans="18:21">
+    <row r="41" spans="18:21" ht="18">
       <c r="R41" s="22"/>
       <c r="S41" s="29"/>
       <c r="T41" s="24"/>
       <c r="U41" s="25"/>
     </row>
-    <row r="42" spans="18:21">
+    <row r="42" spans="18:21" ht="18">
       <c r="R42" s="22"/>
       <c r="S42" s="29"/>
       <c r="T42" s="24"/>
       <c r="U42" s="25"/>
     </row>
-    <row r="43" spans="18:21">
+    <row r="43" spans="18:21" ht="18">
       <c r="R43" s="22"/>
       <c r="S43" s="29"/>
       <c r="T43" s="24"/>
     </row>
-    <row r="44" spans="18:21">
+    <row r="44" spans="18:21" ht="18">
       <c r="R44" s="22"/>
       <c r="S44" s="29"/>
       <c r="T44" s="24"/>
     </row>
-    <row r="45" spans="18:21">
+    <row r="45" spans="18:21" ht="18">
       <c r="R45" s="22"/>
       <c r="S45" s="29"/>
       <c r="T45" s="24"/>
     </row>
-    <row r="46" spans="18:21">
+    <row r="46" spans="18:21" ht="18">
       <c r="R46" s="22"/>
       <c r="S46" s="29"/>
       <c r="T46" s="24"/>
     </row>
-    <row r="47" spans="18:21">
+    <row r="47" spans="18:21" ht="18">
       <c r="R47" s="22"/>
       <c r="S47" s="29"/>
       <c r="T47" s="24"/>
     </row>
-    <row r="48" spans="18:21">
+    <row r="48" spans="18:21" ht="18">
       <c r="R48" s="22"/>
       <c r="S48" s="29"/>
       <c r="T48" s="24"/>
     </row>
-    <row r="49" spans="18:20">
+    <row r="49" spans="18:20" ht="18">
       <c r="R49" s="22"/>
       <c r="S49" s="29"/>
       <c r="T49" s="24"/>
     </row>
-    <row r="50" spans="18:20">
+    <row r="50" spans="18:20" ht="18">
       <c r="R50" s="22"/>
       <c r="S50" s="29"/>
       <c r="T50" s="24"/>
     </row>
-    <row r="51" spans="18:20">
+    <row r="51" spans="18:20" ht="18">
       <c r="R51" s="22"/>
       <c r="S51" s="29"/>
       <c r="T51" s="24"/>
     </row>
-    <row r="52" spans="18:20">
+    <row r="52" spans="18:20" ht="18">
       <c r="R52" s="22"/>
       <c r="S52" s="29"/>
       <c r="T52" s="24"/>
     </row>
-    <row r="53" spans="18:20">
+    <row r="53" spans="18:20" ht="18">
       <c r="R53" s="22"/>
       <c r="S53" s="29"/>
       <c r="T53" s="24"/>
     </row>
-    <row r="54" spans="18:20">
+    <row r="54" spans="18:20" ht="18">
       <c r="R54" s="22"/>
       <c r="S54" s="29"/>
       <c r="T54" s="24"/>
     </row>
-    <row r="55" spans="18:20">
+    <row r="55" spans="18:20" ht="18">
       <c r="R55" s="22"/>
       <c r="S55" s="29"/>
       <c r="T55" s="24"/>
     </row>
-    <row r="56" spans="18:20">
+    <row r="56" spans="18:20" ht="18">
       <c r="R56" s="22"/>
       <c r="S56" s="29"/>
       <c r="T56" s="24"/>
     </row>
-    <row r="57" spans="18:20">
+    <row r="57" spans="18:20" ht="18">
       <c r="R57" s="22"/>
       <c r="S57" s="29"/>
       <c r="T57" s="24"/>
     </row>
-    <row r="58" spans="18:20">
+    <row r="58" spans="18:20" ht="18">
       <c r="R58" s="22"/>
       <c r="S58" s="29"/>
       <c r="T58" s="24"/>
     </row>
-    <row r="59" spans="18:20">
+    <row r="59" spans="18:20" ht="18">
       <c r="R59" s="22"/>
       <c r="S59" s="29"/>
       <c r="T59" s="24"/>
     </row>
-    <row r="60" spans="18:20">
+    <row r="60" spans="18:20" ht="18">
       <c r="R60" s="22"/>
       <c r="S60" s="29"/>
       <c r="T60" s="24"/>
     </row>
-    <row r="61" spans="18:20">
+    <row r="61" spans="18:20" ht="18">
       <c r="R61" s="22"/>
       <c r="S61" s="29"/>
       <c r="T61" s="24"/>
     </row>
-    <row r="62" spans="18:20">
+    <row r="62" spans="18:20" ht="18">
       <c r="R62" s="22"/>
       <c r="S62" s="29"/>
       <c r="T62" s="24"/>
@@ -5164,7 +5164,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" ht="18">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -5200,7 +5200,7 @@
       <c r="T2" s="37"/>
       <c r="U2" s="6"/>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" ht="18">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="E3" s="7"/>
@@ -5243,7 +5243,7 @@
       </c>
       <c r="U3" s="6"/>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" ht="18">
       <c r="A4" s="7"/>
       <c r="B4" s="2" t="s">
         <v>13</v>
@@ -5290,7 +5290,7 @@
       <c r="T4" s="24"/>
       <c r="U4" s="25"/>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" ht="18">
       <c r="A5" s="26"/>
       <c r="B5" s="2" t="s">
         <v>17</v>
@@ -5343,7 +5343,7 @@
       </c>
       <c r="U5" s="25"/>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" ht="18">
       <c r="B6" s="8"/>
       <c r="F6" s="16"/>
       <c r="G6" s="17"/>
@@ -5381,7 +5381,7 @@
       </c>
       <c r="U6" s="25"/>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" ht="18">
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
@@ -5428,7 +5428,7 @@
       </c>
       <c r="U7" s="25"/>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" ht="18">
       <c r="B8" s="8"/>
       <c r="F8" s="16"/>
       <c r="G8" s="28"/>
@@ -5464,7 +5464,7 @@
       </c>
       <c r="U8" s="25"/>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" ht="18">
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
@@ -5509,7 +5509,7 @@
       </c>
       <c r="U9" s="25"/>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" ht="18">
       <c r="B10" s="8"/>
       <c r="F10" s="16"/>
       <c r="G10" s="28"/>
@@ -5545,7 +5545,7 @@
       </c>
       <c r="U10" s="25"/>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" ht="18">
       <c r="B11" s="2" t="s">
         <v>41</v>
       </c>
@@ -5592,7 +5592,7 @@
       </c>
       <c r="U11" s="25"/>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" ht="18">
       <c r="F12" s="16"/>
       <c r="G12" s="28"/>
       <c r="H12" s="5"/>
@@ -5627,7 +5627,7 @@
       </c>
       <c r="U12" s="25"/>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" ht="18">
       <c r="F13" s="16"/>
       <c r="G13" s="28"/>
       <c r="H13" s="5"/>
@@ -5662,7 +5662,7 @@
       </c>
       <c r="U13" s="25"/>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" ht="18">
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -5686,7 +5686,7 @@
       </c>
       <c r="U14" s="25"/>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" ht="18">
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -5710,7 +5710,7 @@
       </c>
       <c r="U15" s="25"/>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" ht="18">
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -5734,7 +5734,7 @@
       </c>
       <c r="U16" s="25"/>
     </row>
-    <row r="17" spans="6:21">
+    <row r="17" spans="6:21" ht="18">
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -5758,7 +5758,7 @@
       </c>
       <c r="U17" s="25"/>
     </row>
-    <row r="18" spans="6:21">
+    <row r="18" spans="6:21" ht="18">
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
@@ -5782,7 +5782,7 @@
       </c>
       <c r="U18" s="25"/>
     </row>
-    <row r="19" spans="6:21">
+    <row r="19" spans="6:21" ht="18">
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -5806,7 +5806,7 @@
       </c>
       <c r="U19" s="25"/>
     </row>
-    <row r="20" spans="6:21">
+    <row r="20" spans="6:21" ht="18">
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
@@ -5830,7 +5830,7 @@
       </c>
       <c r="U20" s="25"/>
     </row>
-    <row r="21" spans="6:21">
+    <row r="21" spans="6:21" ht="18">
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
@@ -5851,7 +5851,7 @@
       </c>
       <c r="U21" s="25"/>
     </row>
-    <row r="22" spans="6:21">
+    <row r="22" spans="6:21" ht="18">
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
@@ -5872,7 +5872,7 @@
       </c>
       <c r="U22" s="25"/>
     </row>
-    <row r="23" spans="6:21">
+    <row r="23" spans="6:21" ht="18">
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="U23" s="25"/>
     </row>
-    <row r="24" spans="6:21">
+    <row r="24" spans="6:21" ht="18">
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
@@ -5914,7 +5914,7 @@
       </c>
       <c r="U24" s="25"/>
     </row>
-    <row r="25" spans="6:21">
+    <row r="25" spans="6:21" ht="18">
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
@@ -5935,7 +5935,7 @@
       </c>
       <c r="U25" s="25"/>
     </row>
-    <row r="26" spans="6:21">
+    <row r="26" spans="6:21" ht="18">
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
@@ -5956,7 +5956,7 @@
       </c>
       <c r="U26" s="25"/>
     </row>
-    <row r="27" spans="6:21">
+    <row r="27" spans="6:21" ht="18">
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
@@ -5977,7 +5977,7 @@
       </c>
       <c r="U27" s="25"/>
     </row>
-    <row r="28" spans="6:21">
+    <row r="28" spans="6:21" ht="18">
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
@@ -5998,7 +5998,7 @@
       </c>
       <c r="U28" s="25"/>
     </row>
-    <row r="29" spans="6:21">
+    <row r="29" spans="6:21" ht="18">
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
@@ -6019,7 +6019,7 @@
       </c>
       <c r="U29" s="25"/>
     </row>
-    <row r="30" spans="6:21">
+    <row r="30" spans="6:21" ht="18">
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
@@ -6040,7 +6040,7 @@
       </c>
       <c r="U30" s="25"/>
     </row>
-    <row r="31" spans="6:21">
+    <row r="31" spans="6:21" ht="18">
       <c r="F31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -6063,7 +6063,7 @@
       </c>
       <c r="U31" s="25"/>
     </row>
-    <row r="32" spans="6:21">
+    <row r="32" spans="6:21" ht="18">
       <c r="R32" s="22">
         <v>210</v>
       </c>
@@ -6075,7 +6075,7 @@
       </c>
       <c r="U32" s="25"/>
     </row>
-    <row r="33" spans="18:21">
+    <row r="33" spans="18:21" ht="18">
       <c r="R33" s="22">
         <v>119</v>
       </c>
@@ -6087,7 +6087,7 @@
       </c>
       <c r="U33" s="25"/>
     </row>
-    <row r="34" spans="18:21">
+    <row r="34" spans="18:21" ht="18">
       <c r="R34" s="22">
         <v>303</v>
       </c>
@@ -6099,7 +6099,7 @@
       </c>
       <c r="U34" s="25"/>
     </row>
-    <row r="35" spans="18:21">
+    <row r="35" spans="18:21" ht="18">
       <c r="R35" s="22">
         <v>47</v>
       </c>
@@ -6111,7 +6111,7 @@
       </c>
       <c r="U35" s="25"/>
     </row>
-    <row r="36" spans="18:21">
+    <row r="36" spans="18:21" ht="18">
       <c r="R36" s="22">
         <v>36</v>
       </c>
@@ -6123,7 +6123,7 @@
       </c>
       <c r="U36" s="25"/>
     </row>
-    <row r="37" spans="18:21">
+    <row r="37" spans="18:21" ht="18">
       <c r="R37" s="22">
         <v>70.599999999999994</v>
       </c>
@@ -6135,7 +6135,7 @@
       </c>
       <c r="U37" s="25"/>
     </row>
-    <row r="38" spans="18:21">
+    <row r="38" spans="18:21" ht="18">
       <c r="R38" s="22">
         <v>100</v>
       </c>
@@ -6147,7 +6147,7 @@
       </c>
       <c r="U38" s="25"/>
     </row>
-    <row r="39" spans="18:21">
+    <row r="39" spans="18:21" ht="18">
       <c r="R39" s="22">
         <v>96</v>
       </c>
@@ -6159,7 +6159,7 @@
       </c>
       <c r="U39" s="25"/>
     </row>
-    <row r="40" spans="18:21">
+    <row r="40" spans="18:21" ht="18">
       <c r="R40" s="22">
         <v>15</v>
       </c>
@@ -6171,7 +6171,7 @@
       </c>
       <c r="U40" s="25"/>
     </row>
-    <row r="41" spans="18:21">
+    <row r="41" spans="18:21" ht="18">
       <c r="R41" s="22">
         <v>366</v>
       </c>
@@ -6183,7 +6183,7 @@
       </c>
       <c r="U41" s="25"/>
     </row>
-    <row r="42" spans="18:21">
+    <row r="42" spans="18:21" ht="18">
       <c r="R42" s="22">
         <v>78</v>
       </c>
@@ -6195,7 +6195,7 @@
       </c>
       <c r="U42" s="25"/>
     </row>
-    <row r="43" spans="18:21">
+    <row r="43" spans="18:21" ht="18">
       <c r="R43" s="22">
         <v>33</v>
       </c>
@@ -6206,7 +6206,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="18:21">
+    <row r="44" spans="18:21" ht="18">
       <c r="R44" s="22">
         <v>447</v>
       </c>
@@ -6217,7 +6217,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="45" spans="18:21">
+    <row r="45" spans="18:21" ht="18">
       <c r="R45" s="22">
         <v>85</v>
       </c>
@@ -6228,7 +6228,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="46" spans="18:21">
+    <row r="46" spans="18:21" ht="18">
       <c r="R46" s="22">
         <v>75</v>
       </c>
@@ -6239,7 +6239,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="47" spans="18:21">
+    <row r="47" spans="18:21" ht="18">
       <c r="R47" s="22">
         <v>73</v>
       </c>
@@ -6250,7 +6250,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="18:21">
+    <row r="48" spans="18:21" ht="18">
       <c r="R48" s="22">
         <v>22</v>
       </c>
@@ -6261,7 +6261,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="18:20">
+    <row r="49" spans="18:20" ht="18">
       <c r="R49" s="22">
         <v>72</v>
       </c>
@@ -6272,7 +6272,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="50" spans="18:20">
+    <row r="50" spans="18:20" ht="18">
       <c r="R50" s="22">
         <v>153</v>
       </c>
@@ -6283,7 +6283,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="51" spans="18:20">
+    <row r="51" spans="18:20" ht="18">
       <c r="R51" s="22">
         <v>86</v>
       </c>
@@ -6294,7 +6294,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="18:20">
+    <row r="52" spans="18:20" ht="18">
       <c r="R52" s="22">
         <v>97</v>
       </c>
@@ -6305,7 +6305,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="18:20">
+    <row r="53" spans="18:20" ht="18">
       <c r="R53" s="22">
         <v>100</v>
       </c>
@@ -6316,7 +6316,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="54" spans="18:20">
+    <row r="54" spans="18:20" ht="18">
       <c r="R54" s="22">
         <v>336</v>
       </c>
@@ -6327,7 +6327,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="18:20">
+    <row r="55" spans="18:20" ht="18">
       <c r="R55" s="22">
         <v>130</v>
       </c>
@@ -6338,7 +6338,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="56" spans="18:20">
+    <row r="56" spans="18:20" ht="18">
       <c r="R56" s="22">
         <v>180</v>
       </c>
@@ -6349,7 +6349,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="57" spans="18:20">
+    <row r="57" spans="18:20" ht="18">
       <c r="R57" s="22">
         <v>72</v>
       </c>
@@ -6360,7 +6360,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="18:20">
+    <row r="58" spans="18:20" ht="18">
       <c r="R58" s="22">
         <v>84</v>
       </c>
@@ -6371,7 +6371,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="59" spans="18:20">
+    <row r="59" spans="18:20" ht="18">
       <c r="R59" s="22">
         <v>73</v>
       </c>
@@ -6382,7 +6382,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="18:20">
+    <row r="60" spans="18:20" ht="18">
       <c r="R60" s="22">
         <v>71</v>
       </c>
@@ -6393,7 +6393,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="61" spans="18:20">
+    <row r="61" spans="18:20" ht="18">
       <c r="R61" s="22">
         <v>133</v>
       </c>
@@ -6404,7 +6404,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="62" spans="18:20">
+    <row r="62" spans="18:20" ht="18">
       <c r="R62" s="22">
         <v>379</v>
       </c>
@@ -6473,7 +6473,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" ht="18">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -6509,7 +6509,7 @@
       <c r="T2" s="37"/>
       <c r="U2" s="6"/>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" ht="18">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="E3" s="7"/>
@@ -6552,7 +6552,7 @@
       </c>
       <c r="U3" s="6"/>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" ht="18">
       <c r="A4" s="7"/>
       <c r="B4" s="2" t="s">
         <v>13</v>
@@ -6599,7 +6599,7 @@
       <c r="T4" s="24"/>
       <c r="U4" s="25"/>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" ht="18">
       <c r="A5" s="26"/>
       <c r="B5" s="2" t="s">
         <v>17</v>
@@ -6652,7 +6652,7 @@
       </c>
       <c r="U5" s="25"/>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" ht="18">
       <c r="B6" s="8"/>
       <c r="F6" s="16"/>
       <c r="G6" s="17"/>
@@ -6690,7 +6690,7 @@
       </c>
       <c r="U6" s="25"/>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" ht="18">
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
@@ -6737,7 +6737,7 @@
       </c>
       <c r="U7" s="25"/>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" ht="18">
       <c r="B8" s="8"/>
       <c r="F8" s="16"/>
       <c r="G8" s="28"/>
@@ -6773,7 +6773,7 @@
       </c>
       <c r="U8" s="25"/>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" ht="18">
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
@@ -6818,7 +6818,7 @@
       </c>
       <c r="U9" s="25"/>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" ht="18">
       <c r="B10" s="8"/>
       <c r="F10" s="16"/>
       <c r="G10" s="28"/>
@@ -6854,7 +6854,7 @@
       </c>
       <c r="U10" s="25"/>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" ht="18">
       <c r="B11" s="2" t="s">
         <v>41</v>
       </c>
@@ -6901,7 +6901,7 @@
       </c>
       <c r="U11" s="25"/>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" ht="18">
       <c r="F12" s="16"/>
       <c r="G12" s="28"/>
       <c r="H12" s="5"/>
@@ -6936,7 +6936,7 @@
       </c>
       <c r="U12" s="25"/>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" ht="18">
       <c r="F13" s="16"/>
       <c r="G13" s="28"/>
       <c r="H13" s="5"/>
@@ -6971,7 +6971,7 @@
       </c>
       <c r="U13" s="25"/>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" ht="18">
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -6995,7 +6995,7 @@
       </c>
       <c r="U14" s="25"/>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" ht="18">
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -7019,7 +7019,7 @@
       </c>
       <c r="U15" s="25"/>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" ht="18">
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -7043,7 +7043,7 @@
       </c>
       <c r="U16" s="25"/>
     </row>
-    <row r="17" spans="6:21">
+    <row r="17" spans="6:21" ht="18">
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -7067,7 +7067,7 @@
       </c>
       <c r="U17" s="25"/>
     </row>
-    <row r="18" spans="6:21">
+    <row r="18" spans="6:21" ht="18">
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
@@ -7091,7 +7091,7 @@
       </c>
       <c r="U18" s="25"/>
     </row>
-    <row r="19" spans="6:21">
+    <row r="19" spans="6:21" ht="18">
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -7115,7 +7115,7 @@
       </c>
       <c r="U19" s="25"/>
     </row>
-    <row r="20" spans="6:21">
+    <row r="20" spans="6:21" ht="18">
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
@@ -7139,7 +7139,7 @@
       </c>
       <c r="U20" s="25"/>
     </row>
-    <row r="21" spans="6:21">
+    <row r="21" spans="6:21" ht="18">
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
@@ -7160,7 +7160,7 @@
       </c>
       <c r="U21" s="25"/>
     </row>
-    <row r="22" spans="6:21">
+    <row r="22" spans="6:21" ht="18">
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
@@ -7181,7 +7181,7 @@
       </c>
       <c r="U22" s="25"/>
     </row>
-    <row r="23" spans="6:21">
+    <row r="23" spans="6:21" ht="18">
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
@@ -7202,7 +7202,7 @@
       </c>
       <c r="U23" s="25"/>
     </row>
-    <row r="24" spans="6:21">
+    <row r="24" spans="6:21" ht="18">
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
@@ -7223,7 +7223,7 @@
       </c>
       <c r="U24" s="25"/>
     </row>
-    <row r="25" spans="6:21">
+    <row r="25" spans="6:21" ht="18">
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
@@ -7244,7 +7244,7 @@
       </c>
       <c r="U25" s="25"/>
     </row>
-    <row r="26" spans="6:21">
+    <row r="26" spans="6:21" ht="18">
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
@@ -7265,7 +7265,7 @@
       </c>
       <c r="U26" s="25"/>
     </row>
-    <row r="27" spans="6:21">
+    <row r="27" spans="6:21" ht="18">
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
@@ -7286,7 +7286,7 @@
       </c>
       <c r="U27" s="25"/>
     </row>
-    <row r="28" spans="6:21">
+    <row r="28" spans="6:21" ht="18">
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
@@ -7307,7 +7307,7 @@
       </c>
       <c r="U28" s="25"/>
     </row>
-    <row r="29" spans="6:21">
+    <row r="29" spans="6:21" ht="18">
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
@@ -7328,7 +7328,7 @@
       </c>
       <c r="U29" s="25"/>
     </row>
-    <row r="30" spans="6:21">
+    <row r="30" spans="6:21" ht="18">
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
@@ -7349,7 +7349,7 @@
       </c>
       <c r="U30" s="25"/>
     </row>
-    <row r="31" spans="6:21">
+    <row r="31" spans="6:21" ht="18">
       <c r="F31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -7372,7 +7372,7 @@
       </c>
       <c r="U31" s="25"/>
     </row>
-    <row r="32" spans="6:21">
+    <row r="32" spans="6:21" ht="18">
       <c r="R32" s="32">
         <v>272</v>
       </c>
@@ -7384,7 +7384,7 @@
       </c>
       <c r="U32" s="25"/>
     </row>
-    <row r="33" spans="18:21">
+    <row r="33" spans="18:21" ht="18">
       <c r="R33" s="32">
         <v>216</v>
       </c>
@@ -7396,7 +7396,7 @@
       </c>
       <c r="U33" s="25"/>
     </row>
-    <row r="34" spans="18:21">
+    <row r="34" spans="18:21" ht="18">
       <c r="R34" s="32">
         <v>103</v>
       </c>
@@ -7408,7 +7408,7 @@
       </c>
       <c r="U34" s="25"/>
     </row>
-    <row r="35" spans="18:21">
+    <row r="35" spans="18:21" ht="18">
       <c r="R35" s="32">
         <v>103</v>
       </c>
@@ -7420,7 +7420,7 @@
       </c>
       <c r="U35" s="25"/>
     </row>
-    <row r="36" spans="18:21">
+    <row r="36" spans="18:21" ht="18">
       <c r="R36" s="32">
         <v>180</v>
       </c>
@@ -7432,7 +7432,7 @@
       </c>
       <c r="U36" s="25"/>
     </row>
-    <row r="37" spans="18:21">
+    <row r="37" spans="18:21" ht="18">
       <c r="R37" s="32">
         <v>222</v>
       </c>
@@ -7444,7 +7444,7 @@
       </c>
       <c r="U37" s="25"/>
     </row>
-    <row r="38" spans="18:21">
+    <row r="38" spans="18:21" ht="18">
       <c r="R38" s="32">
         <v>96</v>
       </c>
@@ -7456,7 +7456,7 @@
       </c>
       <c r="U38" s="25"/>
     </row>
-    <row r="39" spans="18:21">
+    <row r="39" spans="18:21" ht="18">
       <c r="R39" s="32">
         <v>340</v>
       </c>
@@ -7468,7 +7468,7 @@
       </c>
       <c r="U39" s="25"/>
     </row>
-    <row r="40" spans="18:21">
+    <row r="40" spans="18:21" ht="18">
       <c r="R40" s="32">
         <v>215</v>
       </c>
@@ -7480,114 +7480,114 @@
       </c>
       <c r="U40" s="25"/>
     </row>
-    <row r="41" spans="18:21">
+    <row r="41" spans="18:21" ht="18">
       <c r="R41" s="22"/>
       <c r="S41" s="29"/>
       <c r="T41" s="24"/>
       <c r="U41" s="25"/>
     </row>
-    <row r="42" spans="18:21">
+    <row r="42" spans="18:21" ht="18">
       <c r="R42" s="22"/>
       <c r="S42" s="29"/>
       <c r="T42" s="24"/>
       <c r="U42" s="25"/>
     </row>
-    <row r="43" spans="18:21">
+    <row r="43" spans="18:21" ht="18">
       <c r="R43" s="22"/>
       <c r="S43" s="29"/>
       <c r="T43" s="24"/>
     </row>
-    <row r="44" spans="18:21">
+    <row r="44" spans="18:21" ht="18">
       <c r="R44" s="22"/>
       <c r="S44" s="29"/>
       <c r="T44" s="24"/>
     </row>
-    <row r="45" spans="18:21">
+    <row r="45" spans="18:21" ht="18">
       <c r="R45" s="22"/>
       <c r="S45" s="29"/>
       <c r="T45" s="24"/>
     </row>
-    <row r="46" spans="18:21">
+    <row r="46" spans="18:21" ht="18">
       <c r="R46" s="22"/>
       <c r="S46" s="29"/>
       <c r="T46" s="24"/>
     </row>
-    <row r="47" spans="18:21">
+    <row r="47" spans="18:21" ht="18">
       <c r="R47" s="22"/>
       <c r="S47" s="29"/>
       <c r="T47" s="24"/>
     </row>
-    <row r="48" spans="18:21">
+    <row r="48" spans="18:21" ht="18">
       <c r="R48" s="22"/>
       <c r="S48" s="29"/>
       <c r="T48" s="24"/>
     </row>
-    <row r="49" spans="18:20">
+    <row r="49" spans="18:20" ht="18">
       <c r="R49" s="22"/>
       <c r="S49" s="29"/>
       <c r="T49" s="24"/>
     </row>
-    <row r="50" spans="18:20">
+    <row r="50" spans="18:20" ht="18">
       <c r="R50" s="22"/>
       <c r="S50" s="29"/>
       <c r="T50" s="24"/>
     </row>
-    <row r="51" spans="18:20">
+    <row r="51" spans="18:20" ht="18">
       <c r="R51" s="22"/>
       <c r="S51" s="29"/>
       <c r="T51" s="24"/>
     </row>
-    <row r="52" spans="18:20">
+    <row r="52" spans="18:20" ht="18">
       <c r="R52" s="22"/>
       <c r="S52" s="29"/>
       <c r="T52" s="24"/>
     </row>
-    <row r="53" spans="18:20">
+    <row r="53" spans="18:20" ht="18">
       <c r="R53" s="22"/>
       <c r="S53" s="29"/>
       <c r="T53" s="24"/>
     </row>
-    <row r="54" spans="18:20">
+    <row r="54" spans="18:20" ht="18">
       <c r="R54" s="22"/>
       <c r="S54" s="29"/>
       <c r="T54" s="24"/>
     </row>
-    <row r="55" spans="18:20">
+    <row r="55" spans="18:20" ht="18">
       <c r="R55" s="22"/>
       <c r="S55" s="29"/>
       <c r="T55" s="24"/>
     </row>
-    <row r="56" spans="18:20">
+    <row r="56" spans="18:20" ht="18">
       <c r="R56" s="22"/>
       <c r="S56" s="29"/>
       <c r="T56" s="24"/>
     </row>
-    <row r="57" spans="18:20">
+    <row r="57" spans="18:20" ht="18">
       <c r="R57" s="22"/>
       <c r="S57" s="29"/>
       <c r="T57" s="24"/>
     </row>
-    <row r="58" spans="18:20">
+    <row r="58" spans="18:20" ht="18">
       <c r="R58" s="22"/>
       <c r="S58" s="29"/>
       <c r="T58" s="24"/>
     </row>
-    <row r="59" spans="18:20">
+    <row r="59" spans="18:20" ht="18">
       <c r="R59" s="22"/>
       <c r="S59" s="29"/>
       <c r="T59" s="24"/>
     </row>
-    <row r="60" spans="18:20">
+    <row r="60" spans="18:20" ht="18">
       <c r="R60" s="22"/>
       <c r="S60" s="29"/>
       <c r="T60" s="24"/>
     </row>
-    <row r="61" spans="18:20">
+    <row r="61" spans="18:20" ht="18">
       <c r="R61" s="22"/>
       <c r="S61" s="29"/>
       <c r="T61" s="24"/>
     </row>
-    <row r="62" spans="18:20">
+    <row r="62" spans="18:20" ht="18">
       <c r="R62" s="22"/>
       <c r="S62" s="29"/>
       <c r="T62" s="24"/>
@@ -7650,7 +7650,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" ht="18">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -7686,7 +7686,7 @@
       <c r="T2" s="37"/>
       <c r="U2" s="6"/>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" ht="18">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="E3" s="7"/>
@@ -7729,7 +7729,7 @@
       </c>
       <c r="U3" s="6"/>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" ht="18">
       <c r="A4" s="7"/>
       <c r="B4" s="2" t="s">
         <v>13</v>
@@ -7776,7 +7776,7 @@
       <c r="T4" s="24"/>
       <c r="U4" s="25"/>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" ht="18">
       <c r="A5" s="26"/>
       <c r="B5" s="2" t="s">
         <v>17</v>
@@ -7829,7 +7829,7 @@
       </c>
       <c r="U5" s="25"/>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" ht="18">
       <c r="B6" s="8"/>
       <c r="F6" s="16"/>
       <c r="G6" s="17"/>
@@ -7867,7 +7867,7 @@
       </c>
       <c r="U6" s="25"/>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" ht="18">
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
@@ -7914,7 +7914,7 @@
       </c>
       <c r="U7" s="25"/>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" ht="18">
       <c r="B8" s="8"/>
       <c r="F8" s="16"/>
       <c r="G8" s="28"/>
@@ -7950,7 +7950,7 @@
       </c>
       <c r="U8" s="25"/>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" ht="18">
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
@@ -7995,7 +7995,7 @@
       </c>
       <c r="U9" s="25"/>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" ht="18">
       <c r="B10" s="8"/>
       <c r="F10" s="16"/>
       <c r="G10" s="28"/>
@@ -8031,7 +8031,7 @@
       </c>
       <c r="U10" s="25"/>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" ht="18">
       <c r="B11" s="2" t="s">
         <v>41</v>
       </c>
@@ -8078,7 +8078,7 @@
       </c>
       <c r="U11" s="25"/>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" ht="18">
       <c r="F12" s="16"/>
       <c r="G12" s="28"/>
       <c r="H12" s="5"/>
@@ -8113,7 +8113,7 @@
       </c>
       <c r="U12" s="25"/>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" ht="18">
       <c r="F13" s="16"/>
       <c r="G13" s="28"/>
       <c r="H13" s="5"/>
@@ -8148,7 +8148,7 @@
       </c>
       <c r="U13" s="25"/>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" ht="18">
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -8172,7 +8172,7 @@
       </c>
       <c r="U14" s="25"/>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" ht="18">
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -8196,7 +8196,7 @@
       </c>
       <c r="U15" s="25"/>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" ht="18">
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -8220,7 +8220,7 @@
       </c>
       <c r="U16" s="25"/>
     </row>
-    <row r="17" spans="6:21">
+    <row r="17" spans="6:21" ht="18">
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -8244,7 +8244,7 @@
       </c>
       <c r="U17" s="25"/>
     </row>
-    <row r="18" spans="6:21">
+    <row r="18" spans="6:21" ht="18">
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
@@ -8268,7 +8268,7 @@
       </c>
       <c r="U18" s="25"/>
     </row>
-    <row r="19" spans="6:21">
+    <row r="19" spans="6:21" ht="18">
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -8292,7 +8292,7 @@
       </c>
       <c r="U19" s="25"/>
     </row>
-    <row r="20" spans="6:21">
+    <row r="20" spans="6:21" ht="18">
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
@@ -8316,7 +8316,7 @@
       </c>
       <c r="U20" s="25"/>
     </row>
-    <row r="21" spans="6:21">
+    <row r="21" spans="6:21" ht="18">
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
@@ -8337,7 +8337,7 @@
       </c>
       <c r="U21" s="25"/>
     </row>
-    <row r="22" spans="6:21">
+    <row r="22" spans="6:21" ht="18">
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
@@ -8358,7 +8358,7 @@
       </c>
       <c r="U22" s="25"/>
     </row>
-    <row r="23" spans="6:21">
+    <row r="23" spans="6:21" ht="18">
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
@@ -8379,7 +8379,7 @@
       </c>
       <c r="U23" s="25"/>
     </row>
-    <row r="24" spans="6:21">
+    <row r="24" spans="6:21" ht="18">
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
@@ -8400,7 +8400,7 @@
       </c>
       <c r="U24" s="25"/>
     </row>
-    <row r="25" spans="6:21">
+    <row r="25" spans="6:21" ht="18">
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
@@ -8421,7 +8421,7 @@
       </c>
       <c r="U25" s="25"/>
     </row>
-    <row r="26" spans="6:21">
+    <row r="26" spans="6:21" ht="18">
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
@@ -8442,7 +8442,7 @@
       </c>
       <c r="U26" s="25"/>
     </row>
-    <row r="27" spans="6:21">
+    <row r="27" spans="6:21" ht="18">
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
@@ -8463,7 +8463,7 @@
       </c>
       <c r="U27" s="25"/>
     </row>
-    <row r="28" spans="6:21">
+    <row r="28" spans="6:21" ht="18">
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
@@ -8484,7 +8484,7 @@
       </c>
       <c r="U28" s="25"/>
     </row>
-    <row r="29" spans="6:21">
+    <row r="29" spans="6:21" ht="18">
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
@@ -8505,7 +8505,7 @@
       </c>
       <c r="U29" s="25"/>
     </row>
-    <row r="30" spans="6:21">
+    <row r="30" spans="6:21" ht="18">
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
@@ -8526,7 +8526,7 @@
       </c>
       <c r="U30" s="25"/>
     </row>
-    <row r="31" spans="6:21">
+    <row r="31" spans="6:21" ht="18">
       <c r="F31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -8549,7 +8549,7 @@
       </c>
       <c r="U31" s="25"/>
     </row>
-    <row r="32" spans="6:21">
+    <row r="32" spans="6:21" ht="18">
       <c r="R32" s="22">
         <v>40</v>
       </c>
@@ -8561,7 +8561,7 @@
       </c>
       <c r="U32" s="25"/>
     </row>
-    <row r="33" spans="18:21">
+    <row r="33" spans="18:21" ht="18">
       <c r="R33" s="22">
         <v>280</v>
       </c>
@@ -8573,7 +8573,7 @@
       </c>
       <c r="U33" s="25"/>
     </row>
-    <row r="34" spans="18:21">
+    <row r="34" spans="18:21" ht="18">
       <c r="R34" s="22">
         <v>118</v>
       </c>
@@ -8585,7 +8585,7 @@
       </c>
       <c r="U34" s="25"/>
     </row>
-    <row r="35" spans="18:21">
+    <row r="35" spans="18:21" ht="18">
       <c r="R35" s="22">
         <v>146</v>
       </c>
@@ -8597,7 +8597,7 @@
       </c>
       <c r="U35" s="25"/>
     </row>
-    <row r="36" spans="18:21">
+    <row r="36" spans="18:21" ht="18">
       <c r="R36" s="22">
         <v>40</v>
       </c>
@@ -8609,7 +8609,7 @@
       </c>
       <c r="U36" s="25"/>
     </row>
-    <row r="37" spans="18:21">
+    <row r="37" spans="18:21" ht="18">
       <c r="R37" s="22">
         <v>115</v>
       </c>
@@ -8621,7 +8621,7 @@
       </c>
       <c r="U37" s="25"/>
     </row>
-    <row r="38" spans="18:21">
+    <row r="38" spans="18:21" ht="18">
       <c r="R38" s="22">
         <v>276</v>
       </c>
@@ -8633,7 +8633,7 @@
       </c>
       <c r="U38" s="25"/>
     </row>
-    <row r="39" spans="18:21">
+    <row r="39" spans="18:21" ht="18">
       <c r="R39" s="22">
         <v>56</v>
       </c>
@@ -8645,7 +8645,7 @@
       </c>
       <c r="U39" s="25"/>
     </row>
-    <row r="40" spans="18:21">
+    <row r="40" spans="18:21" ht="18">
       <c r="R40" s="22">
         <v>290</v>
       </c>
@@ -8657,7 +8657,7 @@
       </c>
       <c r="U40" s="25"/>
     </row>
-    <row r="41" spans="18:21">
+    <row r="41" spans="18:21" ht="18">
       <c r="R41" s="22">
         <v>70</v>
       </c>
@@ -8669,7 +8669,7 @@
       </c>
       <c r="U41" s="25"/>
     </row>
-    <row r="42" spans="18:21">
+    <row r="42" spans="18:21" ht="18">
       <c r="R42" s="22">
         <v>34</v>
       </c>
@@ -8681,7 +8681,7 @@
       </c>
       <c r="U42" s="25"/>
     </row>
-    <row r="43" spans="18:21">
+    <row r="43" spans="18:21" ht="18">
       <c r="R43" s="22">
         <v>62</v>
       </c>
@@ -8692,7 +8692,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="44" spans="18:21">
+    <row r="44" spans="18:21" ht="18">
       <c r="R44" s="22">
         <v>28</v>
       </c>
@@ -8703,7 +8703,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="45" spans="18:21">
+    <row r="45" spans="18:21" ht="18">
       <c r="R45" s="22">
         <v>52</v>
       </c>
@@ -8714,7 +8714,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="46" spans="18:21">
+    <row r="46" spans="18:21" ht="18">
       <c r="R46" s="22">
         <v>235</v>
       </c>
@@ -8725,7 +8725,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="47" spans="18:21">
+    <row r="47" spans="18:21" ht="18">
       <c r="R47" s="22">
         <v>117</v>
       </c>
@@ -8736,7 +8736,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="18:21">
+    <row r="48" spans="18:21" ht="18">
       <c r="R48" s="22">
         <v>60</v>
       </c>
@@ -8747,7 +8747,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="49" spans="18:20">
+    <row r="49" spans="18:20" ht="18">
       <c r="R49" s="22">
         <v>136</v>
       </c>
@@ -8758,7 +8758,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="50" spans="18:20">
+    <row r="50" spans="18:20" ht="18">
       <c r="R50" s="22">
         <v>395</v>
       </c>
@@ -8769,62 +8769,62 @@
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="18:20">
+    <row r="51" spans="18:20" ht="18">
       <c r="R51" s="22"/>
       <c r="S51" s="29"/>
       <c r="T51" s="24"/>
     </row>
-    <row r="52" spans="18:20">
+    <row r="52" spans="18:20" ht="18">
       <c r="R52" s="22"/>
       <c r="S52" s="29"/>
       <c r="T52" s="24"/>
     </row>
-    <row r="53" spans="18:20">
+    <row r="53" spans="18:20" ht="18">
       <c r="R53" s="22"/>
       <c r="S53" s="29"/>
       <c r="T53" s="24"/>
     </row>
-    <row r="54" spans="18:20">
+    <row r="54" spans="18:20" ht="18">
       <c r="R54" s="22"/>
       <c r="S54" s="29"/>
       <c r="T54" s="24"/>
     </row>
-    <row r="55" spans="18:20">
+    <row r="55" spans="18:20" ht="18">
       <c r="R55" s="22"/>
       <c r="S55" s="29"/>
       <c r="T55" s="24"/>
     </row>
-    <row r="56" spans="18:20">
+    <row r="56" spans="18:20" ht="18">
       <c r="R56" s="22"/>
       <c r="S56" s="29"/>
       <c r="T56" s="24"/>
     </row>
-    <row r="57" spans="18:20">
+    <row r="57" spans="18:20" ht="18">
       <c r="R57" s="22"/>
       <c r="S57" s="29"/>
       <c r="T57" s="24"/>
     </row>
-    <row r="58" spans="18:20">
+    <row r="58" spans="18:20" ht="18">
       <c r="R58" s="22"/>
       <c r="S58" s="29"/>
       <c r="T58" s="24"/>
     </row>
-    <row r="59" spans="18:20">
+    <row r="59" spans="18:20" ht="18">
       <c r="R59" s="22"/>
       <c r="S59" s="29"/>
       <c r="T59" s="24"/>
     </row>
-    <row r="60" spans="18:20">
+    <row r="60" spans="18:20" ht="18">
       <c r="R60" s="22"/>
       <c r="S60" s="29"/>
       <c r="T60" s="24"/>
     </row>
-    <row r="61" spans="18:20">
+    <row r="61" spans="18:20" ht="18">
       <c r="R61" s="22"/>
       <c r="S61" s="29"/>
       <c r="T61" s="24"/>
     </row>
-    <row r="62" spans="18:20">
+    <row r="62" spans="18:20" ht="18">
       <c r="R62" s="22"/>
       <c r="S62" s="29"/>
       <c r="T62" s="24"/>
@@ -8887,7 +8887,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" ht="18">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -8923,7 +8923,7 @@
       <c r="T2" s="37"/>
       <c r="U2" s="6"/>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" ht="18">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="E3" s="7"/>
@@ -8966,7 +8966,7 @@
       </c>
       <c r="U3" s="6"/>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" ht="18">
       <c r="A4" s="7"/>
       <c r="B4" s="2" t="s">
         <v>13</v>
@@ -9013,7 +9013,7 @@
       <c r="T4" s="24"/>
       <c r="U4" s="25"/>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" ht="18">
       <c r="A5" s="26"/>
       <c r="B5" s="2" t="s">
         <v>17</v>
@@ -9062,7 +9062,7 @@
       </c>
       <c r="U5" s="25"/>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" ht="18">
       <c r="B6" s="8"/>
       <c r="F6" s="16"/>
       <c r="G6" s="17"/>
@@ -9100,7 +9100,7 @@
       </c>
       <c r="U6" s="25"/>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" ht="18">
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
@@ -9147,7 +9147,7 @@
       </c>
       <c r="U7" s="25"/>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" ht="18">
       <c r="B8" s="8"/>
       <c r="F8" s="16"/>
       <c r="G8" s="28"/>
@@ -9183,7 +9183,7 @@
       </c>
       <c r="U8" s="25"/>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" ht="18">
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
@@ -9228,7 +9228,7 @@
       </c>
       <c r="U9" s="25"/>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" ht="18">
       <c r="B10" s="8"/>
       <c r="F10" s="16"/>
       <c r="G10" s="28"/>
@@ -9264,7 +9264,7 @@
       </c>
       <c r="U10" s="25"/>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" ht="18">
       <c r="B11" s="2" t="s">
         <v>41</v>
       </c>
@@ -9311,7 +9311,7 @@
       </c>
       <c r="U11" s="25"/>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" ht="18">
       <c r="F12" s="16"/>
       <c r="G12" s="28"/>
       <c r="H12" s="5"/>
@@ -9346,7 +9346,7 @@
       </c>
       <c r="U12" s="25"/>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" ht="18">
       <c r="F13" s="16"/>
       <c r="G13" s="28"/>
       <c r="H13" s="5"/>
@@ -9381,7 +9381,7 @@
       </c>
       <c r="U13" s="25"/>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" ht="18">
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -9405,7 +9405,7 @@
       </c>
       <c r="U14" s="25"/>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" ht="18">
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -9429,7 +9429,7 @@
       </c>
       <c r="U15" s="25"/>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" ht="18">
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -9453,7 +9453,7 @@
       </c>
       <c r="U16" s="25"/>
     </row>
-    <row r="17" spans="6:21">
+    <row r="17" spans="6:21" ht="18">
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -9477,7 +9477,7 @@
       </c>
       <c r="U17" s="25"/>
     </row>
-    <row r="18" spans="6:21">
+    <row r="18" spans="6:21" ht="18">
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
@@ -9501,7 +9501,7 @@
       </c>
       <c r="U18" s="25"/>
     </row>
-    <row r="19" spans="6:21">
+    <row r="19" spans="6:21" ht="18">
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -9525,7 +9525,7 @@
       </c>
       <c r="U19" s="25"/>
     </row>
-    <row r="20" spans="6:21">
+    <row r="20" spans="6:21" ht="18">
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
@@ -9549,7 +9549,7 @@
       </c>
       <c r="U20" s="25"/>
     </row>
-    <row r="21" spans="6:21">
+    <row r="21" spans="6:21" ht="18">
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
@@ -9570,7 +9570,7 @@
       </c>
       <c r="U21" s="25"/>
     </row>
-    <row r="22" spans="6:21">
+    <row r="22" spans="6:21" ht="18">
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
@@ -9591,7 +9591,7 @@
       </c>
       <c r="U22" s="25"/>
     </row>
-    <row r="23" spans="6:21">
+    <row r="23" spans="6:21" ht="18">
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
@@ -9612,7 +9612,7 @@
       </c>
       <c r="U23" s="25"/>
     </row>
-    <row r="24" spans="6:21">
+    <row r="24" spans="6:21" ht="18">
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
@@ -9633,7 +9633,7 @@
       </c>
       <c r="U24" s="25"/>
     </row>
-    <row r="25" spans="6:21">
+    <row r="25" spans="6:21" ht="18">
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
@@ -9654,7 +9654,7 @@
       </c>
       <c r="U25" s="25"/>
     </row>
-    <row r="26" spans="6:21">
+    <row r="26" spans="6:21" ht="18">
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
@@ -9675,7 +9675,7 @@
       </c>
       <c r="U26" s="25"/>
     </row>
-    <row r="27" spans="6:21">
+    <row r="27" spans="6:21" ht="18">
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
@@ -9696,7 +9696,7 @@
       </c>
       <c r="U27" s="25"/>
     </row>
-    <row r="28" spans="6:21">
+    <row r="28" spans="6:21" ht="18">
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
@@ -9717,7 +9717,7 @@
       </c>
       <c r="U28" s="25"/>
     </row>
-    <row r="29" spans="6:21">
+    <row r="29" spans="6:21" ht="18">
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
@@ -9738,7 +9738,7 @@
       </c>
       <c r="U29" s="25"/>
     </row>
-    <row r="30" spans="6:21">
+    <row r="30" spans="6:21" ht="18">
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
@@ -9759,7 +9759,7 @@
       </c>
       <c r="U30" s="25"/>
     </row>
-    <row r="31" spans="6:21">
+    <row r="31" spans="6:21" ht="18">
       <c r="F31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -9782,7 +9782,7 @@
       </c>
       <c r="U31" s="25"/>
     </row>
-    <row r="32" spans="6:21">
+    <row r="32" spans="6:21" ht="18">
       <c r="R32" s="22">
         <v>115</v>
       </c>
@@ -9794,7 +9794,7 @@
       </c>
       <c r="U32" s="25"/>
     </row>
-    <row r="33" spans="18:21">
+    <row r="33" spans="18:21" ht="18">
       <c r="R33" s="22">
         <v>50</v>
       </c>
@@ -9806,7 +9806,7 @@
       </c>
       <c r="U33" s="25"/>
     </row>
-    <row r="34" spans="18:21">
+    <row r="34" spans="18:21" ht="18">
       <c r="R34" s="22">
         <v>390</v>
       </c>
@@ -9818,7 +9818,7 @@
       </c>
       <c r="U34" s="25"/>
     </row>
-    <row r="35" spans="18:21">
+    <row r="35" spans="18:21" ht="18">
       <c r="R35" s="22">
         <v>720</v>
       </c>
@@ -9830,7 +9830,7 @@
       </c>
       <c r="U35" s="25"/>
     </row>
-    <row r="36" spans="18:21">
+    <row r="36" spans="18:21" ht="18">
       <c r="R36" s="22">
         <v>200</v>
       </c>
@@ -9842,7 +9842,7 @@
       </c>
       <c r="U36" s="25"/>
     </row>
-    <row r="37" spans="18:21">
+    <row r="37" spans="18:21" ht="18">
       <c r="R37" s="22">
         <v>94</v>
       </c>
@@ -9854,132 +9854,132 @@
       </c>
       <c r="U37" s="25"/>
     </row>
-    <row r="38" spans="18:21">
+    <row r="38" spans="18:21" ht="18">
       <c r="R38" s="22"/>
       <c r="S38" s="29"/>
       <c r="T38" s="24"/>
       <c r="U38" s="25"/>
     </row>
-    <row r="39" spans="18:21">
+    <row r="39" spans="18:21" ht="18">
       <c r="R39" s="22"/>
       <c r="S39" s="29"/>
       <c r="T39" s="24"/>
       <c r="U39" s="25"/>
     </row>
-    <row r="40" spans="18:21">
+    <row r="40" spans="18:21" ht="18">
       <c r="R40" s="22"/>
       <c r="S40" s="29"/>
       <c r="T40" s="24"/>
       <c r="U40" s="25"/>
     </row>
-    <row r="41" spans="18:21">
+    <row r="41" spans="18:21" ht="18">
       <c r="R41" s="22"/>
       <c r="S41" s="29"/>
       <c r="T41" s="24"/>
       <c r="U41" s="25"/>
     </row>
-    <row r="42" spans="18:21">
+    <row r="42" spans="18:21" ht="18">
       <c r="R42" s="22"/>
       <c r="S42" s="29"/>
       <c r="T42" s="24"/>
       <c r="U42" s="25"/>
     </row>
-    <row r="43" spans="18:21">
+    <row r="43" spans="18:21" ht="18">
       <c r="R43" s="22"/>
       <c r="S43" s="29"/>
       <c r="T43" s="24"/>
     </row>
-    <row r="44" spans="18:21">
+    <row r="44" spans="18:21" ht="18">
       <c r="R44" s="22"/>
       <c r="S44" s="29"/>
       <c r="T44" s="24"/>
     </row>
-    <row r="45" spans="18:21">
+    <row r="45" spans="18:21" ht="18">
       <c r="R45" s="22"/>
       <c r="S45" s="29"/>
       <c r="T45" s="24"/>
     </row>
-    <row r="46" spans="18:21">
+    <row r="46" spans="18:21" ht="18">
       <c r="R46" s="22"/>
       <c r="S46" s="29"/>
       <c r="T46" s="24"/>
     </row>
-    <row r="47" spans="18:21">
+    <row r="47" spans="18:21" ht="18">
       <c r="R47" s="22"/>
       <c r="S47" s="29"/>
       <c r="T47" s="24"/>
     </row>
-    <row r="48" spans="18:21">
+    <row r="48" spans="18:21" ht="18">
       <c r="R48" s="22"/>
       <c r="S48" s="29"/>
       <c r="T48" s="24"/>
     </row>
-    <row r="49" spans="18:20">
+    <row r="49" spans="18:20" ht="18">
       <c r="R49" s="22"/>
       <c r="S49" s="29"/>
       <c r="T49" s="24"/>
     </row>
-    <row r="50" spans="18:20">
+    <row r="50" spans="18:20" ht="18">
       <c r="R50" s="22"/>
       <c r="S50" s="29"/>
       <c r="T50" s="24"/>
     </row>
-    <row r="51" spans="18:20">
+    <row r="51" spans="18:20" ht="18">
       <c r="R51" s="22"/>
       <c r="S51" s="29"/>
       <c r="T51" s="24"/>
     </row>
-    <row r="52" spans="18:20">
+    <row r="52" spans="18:20" ht="18">
       <c r="R52" s="22"/>
       <c r="S52" s="29"/>
       <c r="T52" s="24"/>
     </row>
-    <row r="53" spans="18:20">
+    <row r="53" spans="18:20" ht="18">
       <c r="R53" s="22"/>
       <c r="S53" s="29"/>
       <c r="T53" s="24"/>
     </row>
-    <row r="54" spans="18:20">
+    <row r="54" spans="18:20" ht="18">
       <c r="R54" s="22"/>
       <c r="S54" s="29"/>
       <c r="T54" s="24"/>
     </row>
-    <row r="55" spans="18:20">
+    <row r="55" spans="18:20" ht="18">
       <c r="R55" s="22"/>
       <c r="S55" s="29"/>
       <c r="T55" s="24"/>
     </row>
-    <row r="56" spans="18:20">
+    <row r="56" spans="18:20" ht="18">
       <c r="R56" s="22"/>
       <c r="S56" s="29"/>
       <c r="T56" s="24"/>
     </row>
-    <row r="57" spans="18:20">
+    <row r="57" spans="18:20" ht="18">
       <c r="R57" s="22"/>
       <c r="S57" s="29"/>
       <c r="T57" s="24"/>
     </row>
-    <row r="58" spans="18:20">
+    <row r="58" spans="18:20" ht="18">
       <c r="R58" s="22"/>
       <c r="S58" s="29"/>
       <c r="T58" s="24"/>
     </row>
-    <row r="59" spans="18:20">
+    <row r="59" spans="18:20" ht="18">
       <c r="R59" s="22"/>
       <c r="S59" s="29"/>
       <c r="T59" s="24"/>
     </row>
-    <row r="60" spans="18:20">
+    <row r="60" spans="18:20" ht="18">
       <c r="R60" s="22"/>
       <c r="S60" s="29"/>
       <c r="T60" s="24"/>
     </row>
-    <row r="61" spans="18:20">
+    <row r="61" spans="18:20" ht="18">
       <c r="R61" s="22"/>
       <c r="S61" s="29"/>
       <c r="T61" s="24"/>
     </row>
-    <row r="62" spans="18:20">
+    <row r="62" spans="18:20" ht="18">
       <c r="R62" s="22"/>
       <c r="S62" s="29"/>
       <c r="T62" s="24"/>
@@ -10042,7 +10042,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" ht="18">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -10078,7 +10078,7 @@
       <c r="T2" s="37"/>
       <c r="U2" s="6"/>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" ht="18">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="E3" s="7"/>
@@ -10121,7 +10121,7 @@
       </c>
       <c r="U3" s="6"/>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" ht="18">
       <c r="A4" s="7"/>
       <c r="B4" s="2" t="s">
         <v>13</v>
@@ -10168,7 +10168,7 @@
       <c r="T4" s="24"/>
       <c r="U4" s="25"/>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" ht="18">
       <c r="A5" s="26"/>
       <c r="B5" s="2" t="s">
         <v>17</v>
@@ -10217,7 +10217,7 @@
       </c>
       <c r="U5" s="25"/>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" ht="18">
       <c r="B6" s="8"/>
       <c r="F6" s="16"/>
       <c r="G6" s="17"/>
@@ -10255,7 +10255,7 @@
       </c>
       <c r="U6" s="25"/>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" ht="18">
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
@@ -10302,7 +10302,7 @@
       </c>
       <c r="U7" s="25"/>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" ht="18">
       <c r="B8" s="8"/>
       <c r="F8" s="16"/>
       <c r="G8" s="28"/>
@@ -10338,7 +10338,7 @@
       </c>
       <c r="U8" s="25"/>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" ht="18">
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
@@ -10383,7 +10383,7 @@
       </c>
       <c r="U9" s="25"/>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" ht="18">
       <c r="B10" s="8"/>
       <c r="F10" s="16"/>
       <c r="G10" s="28"/>
@@ -10419,7 +10419,7 @@
       </c>
       <c r="U10" s="25"/>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" ht="18">
       <c r="B11" s="2" t="s">
         <v>41</v>
       </c>
@@ -10466,7 +10466,7 @@
       </c>
       <c r="U11" s="25"/>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" ht="18">
       <c r="F12" s="16"/>
       <c r="G12" s="28"/>
       <c r="H12" s="5"/>
@@ -10501,7 +10501,7 @@
       </c>
       <c r="U12" s="25"/>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" ht="18">
       <c r="F13" s="16"/>
       <c r="G13" s="28"/>
       <c r="H13" s="5"/>
@@ -10536,7 +10536,7 @@
       </c>
       <c r="U13" s="25"/>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" ht="18">
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -10560,7 +10560,7 @@
       </c>
       <c r="U14" s="25"/>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" ht="18">
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -10584,7 +10584,7 @@
       </c>
       <c r="U15" s="25"/>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" ht="18">
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -10608,7 +10608,7 @@
       </c>
       <c r="U16" s="25"/>
     </row>
-    <row r="17" spans="6:21">
+    <row r="17" spans="6:21" ht="18">
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -10632,7 +10632,7 @@
       </c>
       <c r="U17" s="25"/>
     </row>
-    <row r="18" spans="6:21">
+    <row r="18" spans="6:21" ht="18">
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
@@ -10656,7 +10656,7 @@
       </c>
       <c r="U18" s="25"/>
     </row>
-    <row r="19" spans="6:21">
+    <row r="19" spans="6:21" ht="18">
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -10680,7 +10680,7 @@
       </c>
       <c r="U19" s="25"/>
     </row>
-    <row r="20" spans="6:21">
+    <row r="20" spans="6:21" ht="18">
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
@@ -10704,7 +10704,7 @@
       </c>
       <c r="U20" s="25"/>
     </row>
-    <row r="21" spans="6:21">
+    <row r="21" spans="6:21" ht="18">
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
@@ -10725,7 +10725,7 @@
       </c>
       <c r="U21" s="25"/>
     </row>
-    <row r="22" spans="6:21">
+    <row r="22" spans="6:21" ht="18">
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
@@ -10746,7 +10746,7 @@
       </c>
       <c r="U22" s="25"/>
     </row>
-    <row r="23" spans="6:21">
+    <row r="23" spans="6:21" ht="18">
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
@@ -10767,7 +10767,7 @@
       </c>
       <c r="U23" s="25"/>
     </row>
-    <row r="24" spans="6:21">
+    <row r="24" spans="6:21" ht="18">
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
@@ -10788,7 +10788,7 @@
       </c>
       <c r="U24" s="25"/>
     </row>
-    <row r="25" spans="6:21">
+    <row r="25" spans="6:21" ht="18">
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
@@ -10809,7 +10809,7 @@
       </c>
       <c r="U25" s="25"/>
     </row>
-    <row r="26" spans="6:21">
+    <row r="26" spans="6:21" ht="18">
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
@@ -10830,7 +10830,7 @@
       </c>
       <c r="U26" s="25"/>
     </row>
-    <row r="27" spans="6:21">
+    <row r="27" spans="6:21" ht="18">
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
@@ -10851,7 +10851,7 @@
       </c>
       <c r="U27" s="25"/>
     </row>
-    <row r="28" spans="6:21">
+    <row r="28" spans="6:21" ht="18">
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
@@ -10872,7 +10872,7 @@
       </c>
       <c r="U28" s="25"/>
     </row>
-    <row r="29" spans="6:21">
+    <row r="29" spans="6:21" ht="18">
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
@@ -10893,7 +10893,7 @@
       </c>
       <c r="U29" s="25"/>
     </row>
-    <row r="30" spans="6:21">
+    <row r="30" spans="6:21" ht="18">
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
@@ -10914,7 +10914,7 @@
       </c>
       <c r="U30" s="25"/>
     </row>
-    <row r="31" spans="6:21">
+    <row r="31" spans="6:21" ht="18">
       <c r="F31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -10937,7 +10937,7 @@
       </c>
       <c r="U31" s="25"/>
     </row>
-    <row r="32" spans="6:21">
+    <row r="32" spans="6:21" ht="18">
       <c r="R32" s="22">
         <v>18</v>
       </c>
@@ -10949,7 +10949,7 @@
       </c>
       <c r="U32" s="25"/>
     </row>
-    <row r="33" spans="18:21">
+    <row r="33" spans="18:21" ht="18">
       <c r="R33" s="22">
         <v>102</v>
       </c>
@@ -10961,7 +10961,7 @@
       </c>
       <c r="U33" s="25"/>
     </row>
-    <row r="34" spans="18:21">
+    <row r="34" spans="18:21" ht="18">
       <c r="R34" s="22">
         <v>166</v>
       </c>
@@ -10973,7 +10973,7 @@
       </c>
       <c r="U34" s="25"/>
     </row>
-    <row r="35" spans="18:21">
+    <row r="35" spans="18:21" ht="18">
       <c r="R35" s="22">
         <v>110</v>
       </c>
@@ -10985,7 +10985,7 @@
       </c>
       <c r="U35" s="25"/>
     </row>
-    <row r="36" spans="18:21">
+    <row r="36" spans="18:21" ht="18">
       <c r="R36" s="22">
         <v>361</v>
       </c>
@@ -10997,7 +10997,7 @@
       </c>
       <c r="U36" s="25"/>
     </row>
-    <row r="37" spans="18:21">
+    <row r="37" spans="18:21" ht="18">
       <c r="R37" s="22">
         <v>80</v>
       </c>
@@ -11009,7 +11009,7 @@
       </c>
       <c r="U37" s="25"/>
     </row>
-    <row r="38" spans="18:21">
+    <row r="38" spans="18:21" ht="18">
       <c r="R38" s="22">
         <v>395</v>
       </c>
@@ -11021,7 +11021,7 @@
       </c>
       <c r="U38" s="25"/>
     </row>
-    <row r="39" spans="18:21">
+    <row r="39" spans="18:21" ht="18">
       <c r="R39" s="22">
         <v>82</v>
       </c>
@@ -11033,7 +11033,7 @@
       </c>
       <c r="U39" s="25"/>
     </row>
-    <row r="40" spans="18:21">
+    <row r="40" spans="18:21" ht="18">
       <c r="R40" s="22">
         <v>103</v>
       </c>
@@ -11045,7 +11045,7 @@
       </c>
       <c r="U40" s="25"/>
     </row>
-    <row r="41" spans="18:21">
+    <row r="41" spans="18:21" ht="18">
       <c r="R41" s="22">
         <v>268</v>
       </c>
@@ -11057,108 +11057,108 @@
       </c>
       <c r="U41" s="25"/>
     </row>
-    <row r="42" spans="18:21">
+    <row r="42" spans="18:21" ht="18">
       <c r="R42" s="22"/>
       <c r="S42" s="29"/>
       <c r="T42" s="24"/>
       <c r="U42" s="25"/>
     </row>
-    <row r="43" spans="18:21">
+    <row r="43" spans="18:21" ht="18">
       <c r="R43" s="22"/>
       <c r="S43" s="29"/>
       <c r="T43" s="24"/>
     </row>
-    <row r="44" spans="18:21">
+    <row r="44" spans="18:21" ht="18">
       <c r="R44" s="22"/>
       <c r="S44" s="29"/>
       <c r="T44" s="24"/>
     </row>
-    <row r="45" spans="18:21">
+    <row r="45" spans="18:21" ht="18">
       <c r="R45" s="22"/>
       <c r="S45" s="29"/>
       <c r="T45" s="24"/>
     </row>
-    <row r="46" spans="18:21">
+    <row r="46" spans="18:21" ht="18">
       <c r="R46" s="22"/>
       <c r="S46" s="29"/>
       <c r="T46" s="24"/>
     </row>
-    <row r="47" spans="18:21">
+    <row r="47" spans="18:21" ht="18">
       <c r="R47" s="22"/>
       <c r="S47" s="29"/>
       <c r="T47" s="24"/>
     </row>
-    <row r="48" spans="18:21">
+    <row r="48" spans="18:21" ht="18">
       <c r="R48" s="22"/>
       <c r="S48" s="29"/>
       <c r="T48" s="24"/>
     </row>
-    <row r="49" spans="18:20">
+    <row r="49" spans="18:20" ht="18">
       <c r="R49" s="22"/>
       <c r="S49" s="29"/>
       <c r="T49" s="24"/>
     </row>
-    <row r="50" spans="18:20">
+    <row r="50" spans="18:20" ht="18">
       <c r="R50" s="22"/>
       <c r="S50" s="29"/>
       <c r="T50" s="24"/>
     </row>
-    <row r="51" spans="18:20">
+    <row r="51" spans="18:20" ht="18">
       <c r="R51" s="22"/>
       <c r="S51" s="29"/>
       <c r="T51" s="24"/>
     </row>
-    <row r="52" spans="18:20">
+    <row r="52" spans="18:20" ht="18">
       <c r="R52" s="22"/>
       <c r="S52" s="29"/>
       <c r="T52" s="24"/>
     </row>
-    <row r="53" spans="18:20">
+    <row r="53" spans="18:20" ht="18">
       <c r="R53" s="22"/>
       <c r="S53" s="29"/>
       <c r="T53" s="24"/>
     </row>
-    <row r="54" spans="18:20">
+    <row r="54" spans="18:20" ht="18">
       <c r="R54" s="22"/>
       <c r="S54" s="29"/>
       <c r="T54" s="24"/>
     </row>
-    <row r="55" spans="18:20">
+    <row r="55" spans="18:20" ht="18">
       <c r="R55" s="22"/>
       <c r="S55" s="29"/>
       <c r="T55" s="24"/>
     </row>
-    <row r="56" spans="18:20">
+    <row r="56" spans="18:20" ht="18">
       <c r="R56" s="22"/>
       <c r="S56" s="29"/>
       <c r="T56" s="24"/>
     </row>
-    <row r="57" spans="18:20">
+    <row r="57" spans="18:20" ht="18">
       <c r="R57" s="22"/>
       <c r="S57" s="29"/>
       <c r="T57" s="24"/>
     </row>
-    <row r="58" spans="18:20">
+    <row r="58" spans="18:20" ht="18">
       <c r="R58" s="22"/>
       <c r="S58" s="29"/>
       <c r="T58" s="24"/>
     </row>
-    <row r="59" spans="18:20">
+    <row r="59" spans="18:20" ht="18">
       <c r="R59" s="22"/>
       <c r="S59" s="29"/>
       <c r="T59" s="24"/>
     </row>
-    <row r="60" spans="18:20">
+    <row r="60" spans="18:20" ht="18">
       <c r="R60" s="22"/>
       <c r="S60" s="29"/>
       <c r="T60" s="24"/>
     </row>
-    <row r="61" spans="18:20">
+    <row r="61" spans="18:20" ht="18">
       <c r="R61" s="22"/>
       <c r="S61" s="29"/>
       <c r="T61" s="24"/>
     </row>
-    <row r="62" spans="18:20">
+    <row r="62" spans="18:20" ht="18">
       <c r="R62" s="22"/>
       <c r="S62" s="29"/>
       <c r="T62" s="24"/>
@@ -11181,10 +11181,10 @@
   <dimension ref="A1:U62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomRight" activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -11221,7 +11221,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" ht="18">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -11257,7 +11257,7 @@
       <c r="T2" s="37"/>
       <c r="U2" s="6"/>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" ht="18">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="E3" s="7"/>
@@ -11300,7 +11300,7 @@
       </c>
       <c r="U3" s="6"/>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" ht="18">
       <c r="A4" s="7"/>
       <c r="B4" s="2" t="s">
         <v>13</v>
@@ -11347,7 +11347,7 @@
       <c r="T4" s="24"/>
       <c r="U4" s="25"/>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" ht="18">
       <c r="A5" s="26"/>
       <c r="B5" s="2" t="s">
         <v>17</v>
@@ -11400,7 +11400,7 @@
       </c>
       <c r="U5" s="25"/>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" ht="18">
       <c r="B6" s="8"/>
       <c r="F6" s="16"/>
       <c r="G6" s="17"/>
@@ -11438,7 +11438,7 @@
       </c>
       <c r="U6" s="25"/>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" ht="18">
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
@@ -11485,7 +11485,7 @@
       </c>
       <c r="U7" s="25"/>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" ht="18">
       <c r="B8" s="8"/>
       <c r="F8" s="16"/>
       <c r="G8" s="28"/>
@@ -11521,7 +11521,7 @@
       </c>
       <c r="U8" s="25"/>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" ht="18">
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
@@ -11566,7 +11566,7 @@
       </c>
       <c r="U9" s="25"/>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" ht="18">
       <c r="B10" s="8"/>
       <c r="F10" s="16"/>
       <c r="G10" s="28"/>
@@ -11602,7 +11602,7 @@
       </c>
       <c r="U10" s="25"/>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" ht="18">
       <c r="B11" s="2" t="s">
         <v>41</v>
       </c>
@@ -11649,7 +11649,7 @@
       </c>
       <c r="U11" s="25"/>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" ht="18">
       <c r="F12" s="16"/>
       <c r="G12" s="28"/>
       <c r="H12" s="5"/>
@@ -11684,7 +11684,7 @@
       </c>
       <c r="U12" s="25"/>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" ht="18">
       <c r="F13" s="16"/>
       <c r="G13" s="28"/>
       <c r="H13" s="5"/>
@@ -11719,7 +11719,7 @@
       </c>
       <c r="U13" s="25"/>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" ht="18">
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -11743,7 +11743,7 @@
       </c>
       <c r="U14" s="25"/>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" ht="18">
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -11767,7 +11767,7 @@
       </c>
       <c r="U15" s="25"/>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" ht="18">
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -11791,7 +11791,7 @@
       </c>
       <c r="U16" s="25"/>
     </row>
-    <row r="17" spans="6:21">
+    <row r="17" spans="6:21" ht="18">
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -11815,7 +11815,7 @@
       </c>
       <c r="U17" s="25"/>
     </row>
-    <row r="18" spans="6:21">
+    <row r="18" spans="6:21" ht="18">
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
@@ -11839,7 +11839,7 @@
       </c>
       <c r="U18" s="25"/>
     </row>
-    <row r="19" spans="6:21">
+    <row r="19" spans="6:21" ht="18">
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -11863,7 +11863,7 @@
       </c>
       <c r="U19" s="25"/>
     </row>
-    <row r="20" spans="6:21">
+    <row r="20" spans="6:21" ht="18">
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
@@ -11887,7 +11887,7 @@
       </c>
       <c r="U20" s="25"/>
     </row>
-    <row r="21" spans="6:21">
+    <row r="21" spans="6:21" ht="18">
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
@@ -11908,7 +11908,7 @@
       </c>
       <c r="U21" s="25"/>
     </row>
-    <row r="22" spans="6:21">
+    <row r="22" spans="6:21" ht="18">
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
@@ -11929,7 +11929,7 @@
       </c>
       <c r="U22" s="25"/>
     </row>
-    <row r="23" spans="6:21">
+    <row r="23" spans="6:21" ht="18">
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
@@ -11950,7 +11950,7 @@
       </c>
       <c r="U23" s="25"/>
     </row>
-    <row r="24" spans="6:21">
+    <row r="24" spans="6:21" ht="18">
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
@@ -11971,7 +11971,7 @@
       </c>
       <c r="U24" s="25"/>
     </row>
-    <row r="25" spans="6:21">
+    <row r="25" spans="6:21" ht="18">
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
@@ -11992,7 +11992,7 @@
       </c>
       <c r="U25" s="25"/>
     </row>
-    <row r="26" spans="6:21">
+    <row r="26" spans="6:21" ht="18">
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
@@ -12013,7 +12013,7 @@
       </c>
       <c r="U26" s="25"/>
     </row>
-    <row r="27" spans="6:21">
+    <row r="27" spans="6:21" ht="18">
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
@@ -12034,7 +12034,7 @@
       </c>
       <c r="U27" s="25"/>
     </row>
-    <row r="28" spans="6:21">
+    <row r="28" spans="6:21" ht="18">
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
@@ -12055,7 +12055,7 @@
       </c>
       <c r="U28" s="25"/>
     </row>
-    <row r="29" spans="6:21">
+    <row r="29" spans="6:21" ht="18">
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
@@ -12068,15 +12068,15 @@
       <c r="R29" s="22">
         <v>184</v>
       </c>
-      <c r="S29" s="23">
-        <v>44112</v>
+      <c r="S29" s="35" t="s">
+        <v>264</v>
       </c>
       <c r="T29" s="24" t="s">
         <v>266</v>
       </c>
       <c r="U29" s="25"/>
     </row>
-    <row r="30" spans="6:21">
+    <row r="30" spans="6:21" ht="18">
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
@@ -12097,7 +12097,7 @@
       </c>
       <c r="U30" s="25"/>
     </row>
-    <row r="31" spans="6:21">
+    <row r="31" spans="6:21" ht="18">
       <c r="F31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -12120,7 +12120,7 @@
       </c>
       <c r="U31" s="25"/>
     </row>
-    <row r="32" spans="6:21">
+    <row r="32" spans="6:21" ht="18">
       <c r="R32" s="22">
         <v>26</v>
       </c>
@@ -12132,7 +12132,7 @@
       </c>
       <c r="U32" s="25"/>
     </row>
-    <row r="33" spans="18:21">
+    <row r="33" spans="18:21" ht="18">
       <c r="R33" s="22">
         <v>73</v>
       </c>
@@ -12144,7 +12144,7 @@
       </c>
       <c r="U33" s="25"/>
     </row>
-    <row r="34" spans="18:21">
+    <row r="34" spans="18:21" ht="18">
       <c r="R34" s="22">
         <v>50</v>
       </c>
@@ -12156,7 +12156,7 @@
       </c>
       <c r="U34" s="25"/>
     </row>
-    <row r="35" spans="18:21">
+    <row r="35" spans="18:21" ht="18">
       <c r="R35" s="22">
         <v>395</v>
       </c>
@@ -12168,7 +12168,7 @@
       </c>
       <c r="U35" s="25"/>
     </row>
-    <row r="36" spans="18:21">
+    <row r="36" spans="18:21" ht="18">
       <c r="R36" s="22">
         <v>90</v>
       </c>
@@ -12180,7 +12180,7 @@
       </c>
       <c r="U36" s="25"/>
     </row>
-    <row r="37" spans="18:21">
+    <row r="37" spans="18:21" ht="18">
       <c r="R37" s="22">
         <v>191</v>
       </c>
@@ -12192,7 +12192,7 @@
       </c>
       <c r="U37" s="25"/>
     </row>
-    <row r="38" spans="18:21">
+    <row r="38" spans="18:21" ht="18">
       <c r="R38" s="22">
         <v>10</v>
       </c>
@@ -12204,7 +12204,7 @@
       </c>
       <c r="U38" s="25"/>
     </row>
-    <row r="39" spans="18:21">
+    <row r="39" spans="18:21" ht="18">
       <c r="R39" s="22">
         <v>75</v>
       </c>
@@ -12216,7 +12216,7 @@
       </c>
       <c r="U39" s="25"/>
     </row>
-    <row r="40" spans="18:21">
+    <row r="40" spans="18:21" ht="18">
       <c r="R40" s="22">
         <v>130</v>
       </c>
@@ -12228,7 +12228,7 @@
       </c>
       <c r="U40" s="25"/>
     </row>
-    <row r="41" spans="18:21">
+    <row r="41" spans="18:21" ht="18">
       <c r="R41" s="22">
         <v>64</v>
       </c>
@@ -12240,108 +12240,108 @@
       </c>
       <c r="U41" s="25"/>
     </row>
-    <row r="42" spans="18:21">
+    <row r="42" spans="18:21" ht="18">
       <c r="R42" s="22"/>
       <c r="S42" s="29"/>
       <c r="T42" s="24"/>
       <c r="U42" s="25"/>
     </row>
-    <row r="43" spans="18:21">
+    <row r="43" spans="18:21" ht="18">
       <c r="R43" s="22"/>
       <c r="S43" s="29"/>
       <c r="T43" s="24"/>
     </row>
-    <row r="44" spans="18:21">
+    <row r="44" spans="18:21" ht="18">
       <c r="R44" s="22"/>
       <c r="S44" s="29"/>
       <c r="T44" s="24"/>
     </row>
-    <row r="45" spans="18:21">
+    <row r="45" spans="18:21" ht="18">
       <c r="R45" s="22"/>
       <c r="S45" s="29"/>
       <c r="T45" s="24"/>
     </row>
-    <row r="46" spans="18:21">
+    <row r="46" spans="18:21" ht="18">
       <c r="R46" s="22"/>
       <c r="S46" s="29"/>
       <c r="T46" s="24"/>
     </row>
-    <row r="47" spans="18:21">
+    <row r="47" spans="18:21" ht="18">
       <c r="R47" s="22"/>
       <c r="S47" s="29"/>
       <c r="T47" s="24"/>
     </row>
-    <row r="48" spans="18:21">
+    <row r="48" spans="18:21" ht="18">
       <c r="R48" s="22"/>
       <c r="S48" s="29"/>
       <c r="T48" s="24"/>
     </row>
-    <row r="49" spans="18:20">
+    <row r="49" spans="18:20" ht="18">
       <c r="R49" s="22"/>
       <c r="S49" s="29"/>
       <c r="T49" s="24"/>
     </row>
-    <row r="50" spans="18:20">
+    <row r="50" spans="18:20" ht="18">
       <c r="R50" s="22"/>
       <c r="S50" s="29"/>
       <c r="T50" s="24"/>
     </row>
-    <row r="51" spans="18:20">
+    <row r="51" spans="18:20" ht="18">
       <c r="R51" s="22"/>
       <c r="S51" s="29"/>
       <c r="T51" s="24"/>
     </row>
-    <row r="52" spans="18:20">
+    <row r="52" spans="18:20" ht="18">
       <c r="R52" s="22"/>
       <c r="S52" s="29"/>
       <c r="T52" s="24"/>
     </row>
-    <row r="53" spans="18:20">
+    <row r="53" spans="18:20" ht="18">
       <c r="R53" s="22"/>
       <c r="S53" s="29"/>
       <c r="T53" s="24"/>
     </row>
-    <row r="54" spans="18:20">
+    <row r="54" spans="18:20" ht="18">
       <c r="R54" s="22"/>
       <c r="S54" s="29"/>
       <c r="T54" s="24"/>
     </row>
-    <row r="55" spans="18:20">
+    <row r="55" spans="18:20" ht="18">
       <c r="R55" s="22"/>
       <c r="S55" s="29"/>
       <c r="T55" s="24"/>
     </row>
-    <row r="56" spans="18:20">
+    <row r="56" spans="18:20" ht="18">
       <c r="R56" s="22"/>
       <c r="S56" s="29"/>
       <c r="T56" s="24"/>
     </row>
-    <row r="57" spans="18:20">
+    <row r="57" spans="18:20" ht="18">
       <c r="R57" s="22"/>
       <c r="S57" s="29"/>
       <c r="T57" s="24"/>
     </row>
-    <row r="58" spans="18:20">
+    <row r="58" spans="18:20" ht="18">
       <c r="R58" s="22"/>
       <c r="S58" s="29"/>
       <c r="T58" s="24"/>
     </row>
-    <row r="59" spans="18:20">
+    <row r="59" spans="18:20" ht="18">
       <c r="R59" s="22"/>
       <c r="S59" s="29"/>
       <c r="T59" s="24"/>
     </row>
-    <row r="60" spans="18:20">
+    <row r="60" spans="18:20" ht="18">
       <c r="R60" s="22"/>
       <c r="S60" s="29"/>
       <c r="T60" s="24"/>
     </row>
-    <row r="61" spans="18:20">
+    <row r="61" spans="18:20" ht="18">
       <c r="R61" s="22"/>
       <c r="S61" s="29"/>
       <c r="T61" s="24"/>
     </row>
-    <row r="62" spans="18:20">
+    <row r="62" spans="18:20" ht="18">
       <c r="R62" s="22"/>
       <c r="S62" s="29"/>
       <c r="T62" s="24"/>

</xml_diff>